<commit_message>
added dedicated prediction output window to client GUI, edited ML model script to display training time
</commit_message>
<xml_diff>
--- a/ML_Model_Scripts/Performance Data/New performance data.xlsx
+++ b/ML_Model_Scripts/Performance Data/New performance data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\vivs\Documents\concreteml-covid-classifier\ML_Model_Scripts\Performance Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D274D03-5FD2-4CC4-9668-57EF6189227B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420D46A5-4B13-43D5-9B66-7DDC96A1A745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Plaintext</t>
   </si>
@@ -120,6 +120,21 @@
   </si>
   <si>
     <t>*note: refer to PNG files for confusion matrix results</t>
+  </si>
+  <si>
+    <t>training time (seconds)</t>
+  </si>
+  <si>
+    <t>number of training iterations</t>
+  </si>
+  <si>
+    <t>100 (default iterations)</t>
+  </si>
+  <si>
+    <t>training_time</t>
+  </si>
+  <si>
+    <t>training time vs plaintext</t>
   </si>
 </sst>
 </file>
@@ -127,7 +142,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.00000%"/>
+    <numFmt numFmtId="164" formatCode="0.00000%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -184,7 +199,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -233,11 +248,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -257,17 +296,35 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -276,45 +333,45 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="17">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -341,6 +398,40 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -377,34 +468,6 @@
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -419,31 +482,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{394116DB-3FC4-462F-A6EA-93CE28E8DEFC}" name="Table1" displayName="Table1" ref="A2:C12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A2:C12" xr:uid="{394116DB-3FC4-462F-A6EA-93CE28E8DEFC}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{394116DB-3FC4-462F-A6EA-93CE28E8DEFC}" name="Table1" displayName="Table1" ref="A2:D12" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A2:D12" xr:uid="{394116DB-3FC4-462F-A6EA-93CE28E8DEFC}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{CFED003A-DA1B-4CE5-8524-E8936E3DBC3E}" name="accuracy" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{E1948511-7D29-400B-AA26-A9E601B91AEC}" name="roc_auc_score" dataDxfId="13"/>
     <tableColumn id="3" xr3:uid="{7A51BA68-3B03-403B-89BD-9395BC2871EB}" name="test_set_prediction_time" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{832497D3-116A-4DE3-A927-E67DAAF345F9}" name="training_time" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{51C47605-6D87-4135-B9CB-CCDCB9C5785B}" name="Table2" displayName="Table2" ref="A2:C12" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A2:C12" xr:uid="{51C47605-6D87-4135-B9CB-CCDCB9C5785B}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{51C47605-6D87-4135-B9CB-CCDCB9C5785B}" name="Table2" displayName="Table2" ref="A2:D12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A2:D12" xr:uid="{51C47605-6D87-4135-B9CB-CCDCB9C5785B}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D1463535-C8C0-4CDA-8D2E-CC2600120E02}" name="accuracy" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{B5EFEA31-5244-404F-A004-FB2C24EF05C5}" name="roc_auc_score" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{4ECC1606-A197-4F05-B01C-AE05A7881542}" name="test_set_prediction_time" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{5607816E-855A-4944-AF8F-D298454F5A6B}" name="training_time" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{274CBF2D-66AB-4A51-A1D7-B37000717CE9}" name="Table3" displayName="Table3" ref="A2:C12" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{274CBF2D-66AB-4A51-A1D7-B37000717CE9}" name="Table3" displayName="Table3" ref="A2:C12" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A2:C12" xr:uid="{274CBF2D-66AB-4A51-A1D7-B37000717CE9}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{CF2700D2-A674-464D-946D-1F615B6D91A7}" name="accuracy" dataDxfId="4"/>
@@ -717,133 +782,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:J20"/>
+  <dimension ref="A3:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="31.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="18.5546875" style="1"/>
+    <col min="6" max="6" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="25.21875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="18.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="12" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="12" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="D5" s="19"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="13"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="13"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="D7" s="19"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="7" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="15"/>
+      <c r="B13" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="19" t="s">
+      <c r="C13" s="14"/>
+      <c r="D13" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="21" t="s">
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="22"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="15"/>
       <c r="B14" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="H14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="22" t="s">
+      <c r="I14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="22" t="s">
+      <c r="J14" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="22"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
@@ -863,25 +934,32 @@
         <f>D15/$A$20</f>
         <v>1.501139125641707E-7</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="5">
+        <f>AVERAGE(Table1[training_time])</f>
+        <v>9.5986247062682842E-2</v>
+      </c>
+      <c r="G15" s="11">
         <f>ABS(B15-$B$15)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="23">
+      <c r="H15" s="11">
         <f>ABS(1-C15/$C$15)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="4">
+      <c r="I15" s="4">
         <f>ABS(1-D15/$D$15)</f>
         <v>0</v>
       </c>
-      <c r="I15" s="6" t="str">
-        <f>ROUND((H15)+1,2) &amp; "x slower"</f>
+      <c r="J15" s="4">
+        <f>ABS(1-(F15/$F$15))</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="6" t="str">
+        <f>ROUND((I15)+1,2) &amp; "x slower"</f>
         <v>1x slower</v>
       </c>
-      <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
@@ -901,25 +979,32 @@
         <f>D16/$A$20</f>
         <v>4.6055393315487209E-7</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="5">
+        <f>AVERAGE(Table2[training_time])</f>
+        <v>0.1156843423843382</v>
+      </c>
+      <c r="G16" s="11">
         <f>ABS(B16-$B$15)</f>
         <v>9.5559302979209004E-4</v>
       </c>
-      <c r="G16" s="23">
+      <c r="H16" s="11">
         <f>ABS(1-C16/$C$15)</f>
         <v>1.3146976477473871E-5</v>
       </c>
-      <c r="H16" s="4">
+      <c r="I16" s="4">
         <f>ABS(1-D16/$D$15)</f>
         <v>2.068029640210693</v>
       </c>
-      <c r="I16" s="6" t="str">
-        <f t="shared" ref="I16:J17" si="0">ROUND((H16)+1,2) &amp; "x slower"</f>
+      <c r="J16" s="4">
+        <f>ABS(1-(F16/$F$15))</f>
+        <v>0.20521789240068644</v>
+      </c>
+      <c r="K16" s="6" t="str">
+        <f>ROUND((I16)+1,2) &amp; "x slower"</f>
         <v>3.07x slower</v>
       </c>
-      <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
@@ -939,50 +1024,68 @@
         <f>D17/$A$20</f>
         <v>5.3706498813468201E-7</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="5">
+        <f>AVERAGE(Table2[training_time])</f>
+        <v>0.1156843423843382</v>
+      </c>
+      <c r="G17" s="11">
         <f>ABS(B17-$B$15)</f>
         <v>1.0680157391793621E-3</v>
       </c>
-      <c r="G17" s="23">
+      <c r="H17" s="11">
         <f>ABS(1-C17/$C$15)</f>
         <v>8.3487174835639166E-6</v>
       </c>
-      <c r="H17" s="4">
+      <c r="I17" s="4">
         <f>ABS(1-D17/$D$15)</f>
         <v>2.5777162753325573</v>
       </c>
-      <c r="I17" s="6" t="str">
-        <f t="shared" si="0"/>
+      <c r="J17" s="4">
+        <f>ABS(1-(F17/$F$15))</f>
+        <v>0.20521789240068644</v>
+      </c>
+      <c r="K17" s="6" t="str">
+        <f>ROUND((I17)+1,2) &amp; "x slower"</f>
         <v>3.58x slower</v>
       </c>
-      <c r="J17" s="6"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>1779</v>
       </c>
     </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A3:D3"/>
+  <mergeCells count="15">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="D13:F13"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="A13:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -991,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{866B64C5-BF1A-499D-83A6-EB0DDBB99A75}">
-  <dimension ref="A2:C21"/>
+  <dimension ref="A2:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1002,137 +1105,170 @@
     <col min="3" max="3" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="17">
+      <c r="D2" s="24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>0.98763350196739697</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="1">
         <v>0.99660712684762598</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="1">
         <v>2.13384628295898E-4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="17">
+      <c r="D3" s="23">
+        <v>0.117744445800781</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>0.98819561551433399</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="1">
         <v>0.996539459835875</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="1">
         <v>4.2676925659179601E-4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="17">
+      <c r="D4" s="23">
+        <v>0.11230659484863199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>0.98819561551433399</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="1">
         <v>0.99656215130963099</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="1">
         <v>3.5905838012695302E-4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="17">
+      <c r="D5" s="23">
+        <v>0.14333224296569799</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>0.98988195615514296</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="1">
         <v>0.99648901165327697</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="1">
         <v>1.9264221191406201E-4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="17">
+      <c r="D6" s="23">
+        <v>7.5737237930297796E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>0.98763350196739697</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="1">
         <v>0.99660461352584695</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="1">
         <v>2.5749206542968701E-4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="17">
+      <c r="D7" s="23">
+        <v>8.4540605545043904E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>0.98988195615514296</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="1">
         <v>0.99659926717143699</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="1">
         <v>1.8930435180664E-4</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="17">
+      <c r="D8" s="23">
+        <v>7.9212427139282199E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>0.98707138842046005</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="1">
         <v>0.99667628669468999</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="1">
         <v>2.6893615722656201E-4</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="17">
+      <c r="D9" s="23">
+        <v>7.4156761169433594E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
         <v>0.98988195615514296</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="1">
         <v>0.996591862758198</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="1">
         <v>2.5749206542968701E-4</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="17">
+      <c r="D10" s="23">
+        <v>8.7489604949951102E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
         <v>0.98538504777965097</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="1">
         <v>0.99660694710886499</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="1">
         <v>2.5749206542968701E-4</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="17">
+      <c r="D11" s="23">
+        <v>0.10050606727600001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
         <v>0.98931984260820605</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="1">
         <v>0.99660603648084101</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="1">
         <v>2.47955322265625E-4</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" s="23">
+        <v>8.4836483001708901E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
@@ -1161,10 +1297,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82957BC5-845A-415D-A9C1-AC076A441DA7}">
-  <dimension ref="A2:C12"/>
+  <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1173,7 +1309,7 @@
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1183,8 +1319,11 @@
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0.98819561551433399</v>
       </c>
@@ -1194,8 +1333,11 @@
       <c r="C3" s="1">
         <v>1.3179779052734299E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="1">
+        <v>0.111749172210693</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>0.99044406970207899</v>
       </c>
@@ -1205,8 +1347,11 @@
       <c r="C4" s="1">
         <v>5.3310394287109299E-4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="1">
+        <v>0.113413095474243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>0.98482293423271505</v>
       </c>
@@ -1216,8 +1361,11 @@
       <c r="C5" s="1">
         <v>6.0558319091796799E-4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="1">
+        <v>0.11999559402465799</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>0.98482293423271505</v>
       </c>
@@ -1227,8 +1375,11 @@
       <c r="C6" s="1">
         <v>6.9093704223632802E-4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="1">
+        <v>0.11184048652648899</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>0.99213041034288896</v>
       </c>
@@ -1238,8 +1389,11 @@
       <c r="C7" s="1">
         <v>6.3920021057128895E-4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="1">
+        <v>0.129948616027832</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>0.98707138842046005</v>
       </c>
@@ -1249,8 +1403,11 @@
       <c r="C8" s="1">
         <v>9.7990036010742101E-4</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="1">
+        <v>0.10836601257324199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>0.98650927487352402</v>
       </c>
@@ -1260,8 +1417,11 @@
       <c r="C9" s="1">
         <v>5.5932998657226497E-4</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" s="1">
+        <v>0.110030174255371</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>0.98538504777965097</v>
       </c>
@@ -1271,8 +1431,11 @@
       <c r="C10" s="1">
         <v>1.8444061279296799E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="1">
+        <v>0.114490270614624</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>0.98707138842046005</v>
       </c>
@@ -1282,8 +1445,11 @@
       <c r="C11" s="1">
         <v>5.2356719970703103E-4</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" s="1">
+        <v>0.117451429367065</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>0.98707138842046005</v>
       </c>
@@ -1292,6 +1458,9 @@
       </c>
       <c r="C12" s="1">
         <v>4.9924850463867101E-4</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.119558572769165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added key size and data size comparisons in app (printed to terminal as of the moment) + new performance data
</commit_message>
<xml_diff>
--- a/ML_Model_Scripts/Performance Data/New performance data.xlsx
+++ b/ML_Model_Scripts/Performance Data/New performance data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\vivs\Documents\concreteml-covid-classifier\ML_Model_Scripts\Performance Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420D46A5-4B13-43D5-9B66-7DDC96A1A745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37C101F-3590-4BE6-9289-852DF0288554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
     <sheet name="scikit-learn" sheetId="2" r:id="rId2"/>
     <sheet name="quantized plaintext" sheetId="3" r:id="rId3"/>
-    <sheet name="fhe" sheetId="4" r:id="rId4"/>
+    <sheet name="fhe (+ sizes)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>Plaintext</t>
   </si>
@@ -135,14 +135,69 @@
   </si>
   <si>
     <t>training time vs plaintext</t>
+  </si>
+  <si>
+    <t>Model Type</t>
+  </si>
+  <si>
+    <t>Linear Regression</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>SVC</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>Run no.</t>
+  </si>
+  <si>
+    <t>Plaintext Size (kB)</t>
+  </si>
+  <si>
+    <t>Ciphertext Size (kB)</t>
+  </si>
+  <si>
+    <t>Percentage Increase</t>
+  </si>
+  <si>
+    <t>Eval Key Size (kB)</t>
+  </si>
+  <si>
+    <t>Private Key Size (kB)</t>
+  </si>
+  <si>
+    <t>Strain</t>
+  </si>
+  <si>
+    <t>B.1.1.529 (Omicron)</t>
+  </si>
+  <si>
+    <t>B.1.617.2 (Delta)</t>
+  </si>
+  <si>
+    <t>C.37 (Lambda)</t>
+  </si>
+  <si>
+    <t>B.1.621 (Mu)</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000%"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -276,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -309,59 +364,166 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="38">
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -372,38 +534,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -482,38 +612,86 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{394116DB-3FC4-462F-A6EA-93CE28E8DEFC}" name="Table1" displayName="Table1" ref="A2:D12" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{394116DB-3FC4-462F-A6EA-93CE28E8DEFC}" name="Table1" displayName="Table1" ref="A2:D12" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <autoFilter ref="A2:D12" xr:uid="{394116DB-3FC4-462F-A6EA-93CE28E8DEFC}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CFED003A-DA1B-4CE5-8524-E8936E3DBC3E}" name="accuracy" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{E1948511-7D29-400B-AA26-A9E601B91AEC}" name="roc_auc_score" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{7A51BA68-3B03-403B-89BD-9395BC2871EB}" name="test_set_prediction_time" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{832497D3-116A-4DE3-A927-E67DAAF345F9}" name="training_time" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{CFED003A-DA1B-4CE5-8524-E8936E3DBC3E}" name="accuracy" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{E1948511-7D29-400B-AA26-A9E601B91AEC}" name="roc_auc_score" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{7A51BA68-3B03-403B-89BD-9395BC2871EB}" name="test_set_prediction_time" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{832497D3-116A-4DE3-A927-E67DAAF345F9}" name="training_time" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{51C47605-6D87-4135-B9CB-CCDCB9C5785B}" name="Table2" displayName="Table2" ref="A2:D12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A2:D12" xr:uid="{51C47605-6D87-4135-B9CB-CCDCB9C5785B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4BDC63FC-A3D1-4A76-971A-2D7E1A53E2E0}" name="Table5" displayName="Table5" ref="F2:I12" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+  <autoFilter ref="F2:I12" xr:uid="{4BDC63FC-A3D1-4A76-971A-2D7E1A53E2E0}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D1463535-C8C0-4CDA-8D2E-CC2600120E02}" name="accuracy" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{B5EFEA31-5244-404F-A004-FB2C24EF05C5}" name="roc_auc_score" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{4ECC1606-A197-4F05-B01C-AE05A7881542}" name="test_set_prediction_time" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{5607816E-855A-4944-AF8F-D298454F5A6B}" name="training_time" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{590571B2-7F3A-4AB4-82F6-490D3ABC5319}" name="Linear Regression" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{07D40D9A-323F-4837-9150-E888FA1F58E4}" name="Random Forest" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{852582AB-50FA-439E-807C-CDA24D4C70C4}" name="SVC" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{799C5940-B5F5-4EC3-89E0-C94AD8F231A7}" name="Logistic Regression" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{274CBF2D-66AB-4A51-A1D7-B37000717CE9}" name="Table3" displayName="Table3" ref="A2:C12" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{51C47605-6D87-4135-B9CB-CCDCB9C5785B}" name="Table2" displayName="Table2" ref="A2:D12" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A2:D12" xr:uid="{51C47605-6D87-4135-B9CB-CCDCB9C5785B}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{D1463535-C8C0-4CDA-8D2E-CC2600120E02}" name="accuracy" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{B5EFEA31-5244-404F-A004-FB2C24EF05C5}" name="roc_auc_score" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{4ECC1606-A197-4F05-B01C-AE05A7881542}" name="test_set_prediction_time" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{5607816E-855A-4944-AF8F-D298454F5A6B}" name="training_time" dataDxfId="20"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E7F5510B-26CB-48F1-9BD1-CC49FC0D68B6}" name="Table57" displayName="Table57" ref="F2:I12" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="F2:I12" xr:uid="{E7F5510B-26CB-48F1-9BD1-CC49FC0D68B6}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{E9413FF7-271E-469E-BCC5-DC52D55F3A3A}" name="Linear Regression" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{D6DB89F1-F914-4459-8D10-40E13FB298B0}" name="Random Forest" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{C4F7B31F-A9DC-4D0B-B72F-83D8E4B839D1}" name="SVC" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{546CB1C7-04D1-48CD-81F4-0F71D956336F}" name="Logistic Regression" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{274CBF2D-66AB-4A51-A1D7-B37000717CE9}" name="Table3" displayName="Table3" ref="A2:C12" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A2:C12" xr:uid="{274CBF2D-66AB-4A51-A1D7-B37000717CE9}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{CF2700D2-A674-464D-946D-1F615B6D91A7}" name="accuracy" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{2EA8A39C-2C3A-4F0F-9292-AEF706305A49}" name="roc_auc_score" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{C2D54946-E516-44E8-911A-9CDEC9118CD9}" name="test_set_prediction_time" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{CF2700D2-A674-464D-946D-1F615B6D91A7}" name="accuracy" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{2EA8A39C-2C3A-4F0F-9292-AEF706305A49}" name="roc_auc_score" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{C2D54946-E516-44E8-911A-9CDEC9118CD9}" name="test_set_prediction_time" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E5D7C54E-16E1-4754-8032-313998CAF65E}" name="Table4" displayName="Table4" ref="A14:G20" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A14:G20" xr:uid="{E5D7C54E-16E1-4754-8032-313998CAF65E}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{E078801A-15C7-4980-8156-8BD235967CEF}" name="Run no." dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{EFC1765B-5F55-4EA2-8F83-E8A7E7C44F75}" name="Strain" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{F62F3C7A-45AD-49AC-B959-B08E20AA523B}" name="Plaintext Size (kB)" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{C782FB93-D156-4C46-B517-3AE650180077}" name="Ciphertext Size (kB)" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{F4080A86-E0E6-428D-9973-84C9B618A1A8}" name="Percentage Increase" dataDxfId="2">
+      <calculatedColumnFormula>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{30A9C073-FC8D-4D3E-B3F4-A25F0535FC84}" name="Eval Key Size (kB)" dataDxfId="1">
+      <calculatedColumnFormula>0.023</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{9EE40A62-0BC7-4513-9103-444B1C53E933}" name="Private Key Size (kB)" dataDxfId="0">
+      <calculatedColumnFormula>(Table4[[#This Row],[Run no.]]/Table4[[#This Row],[Percentage Increase]])*100</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -782,17 +960,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:K22"/>
+  <dimension ref="A3:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.77734375" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
@@ -802,12 +980,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -815,64 +993,64 @@
       <c r="I3" s="8"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="18" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="19"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="19"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="19"/>
+      <c r="D6" s="17"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="19"/>
+      <c r="D7" s="17"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="14" t="s">
+      <c r="A13" s="26"/>
+      <c r="B13" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="13" t="s">
+      <c r="C13" s="25"/>
+      <c r="D13" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
       <c r="G13" s="20" t="s">
         <v>7</v>
       </c>
@@ -882,7 +1060,7 @@
       <c r="K13" s="22"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="3" t="s">
         <v>3</v>
       </c>
@@ -895,7 +1073,7 @@
       <c r="E14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="27" t="s">
+      <c r="F14" s="12" t="s">
         <v>27</v>
       </c>
       <c r="G14" s="10" t="s">
@@ -1009,15 +1187,15 @@
         <v>2</v>
       </c>
       <c r="B17" s="4">
-        <f>AVERAGE(fhe!A3:A12)</f>
+        <f>AVERAGE('fhe (+ sizes)'!A3:A12)</f>
         <v>0.98724002248454146</v>
       </c>
       <c r="C17" s="5">
-        <f>AVERAGE(fhe!B3:B12)</f>
+        <f>AVERAGE('fhe (+ sizes)'!B3:B12)</f>
         <v>0.9965799561046621</v>
       </c>
       <c r="D17" s="5">
-        <f>AVERAGE(fhe!C3:C12)</f>
+        <f>AVERAGE('fhe (+ sizes)'!C3:C12)</f>
         <v>9.5543861389159931E-4</v>
       </c>
       <c r="E17" s="5">
@@ -1067,6 +1245,65 @@
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="5">
+        <f>AVERAGE(Table5[Linear Regression])</f>
+        <v>95.709265309573439</v>
+      </c>
+      <c r="C25" s="5">
+        <f>AVERAGE(Table5[Random Forest])</f>
+        <v>98.684654300168589</v>
+      </c>
+      <c r="D25" s="5">
+        <f>AVERAGE(Table5[SVC])</f>
+        <v>98.532883642495747</v>
+      </c>
+      <c r="E25" s="5">
+        <f>AVERAGE(Table5[Logistic Regression])</f>
+        <v>98.740865654862233</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="5">
+        <f>AVERAGE(Table57[Linear Regression])</f>
+        <v>95.556837638640559</v>
+      </c>
+      <c r="C26" s="5">
+        <f>AVERAGE(Table57[Random Forest])</f>
+        <v>98.010118043844813</v>
+      </c>
+      <c r="D26" s="5">
+        <f>AVERAGE(Table57[SVC])</f>
+        <v>98.577852726250654</v>
+      </c>
+      <c r="E26" s="5">
+        <f>AVERAGE(Table57[Logistic Regression])</f>
+        <v>98.72962338392351</v>
       </c>
     </row>
   </sheetData>
@@ -1077,15 +1314,15 @@
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="G13:K13"/>
     <mergeCell ref="D13:F13"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="A13:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1094,10 +1331,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{866B64C5-BF1A-499D-83A6-EB0DDBB99A75}">
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I2" sqref="I2:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1105,7 +1342,7 @@
     <col min="3" max="3" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
@@ -1115,11 +1352,23 @@
       <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0.98763350196739697</v>
       </c>
@@ -1129,11 +1378,23 @@
       <c r="C3" s="1">
         <v>2.13384628295898E-4</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="1">
         <v>0.117744445800781</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F3" s="13">
+        <v>95.7917644096283</v>
+      </c>
+      <c r="G3" s="13">
+        <v>98.763350196739694</v>
+      </c>
+      <c r="H3" s="13">
+        <v>98.763350196739694</v>
+      </c>
+      <c r="I3" s="1">
+        <v>98.650927487352405</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>0.98819561551433399</v>
       </c>
@@ -1143,11 +1404,23 @@
       <c r="C4" s="1">
         <v>4.2676925659179601E-4</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="1">
         <v>0.11230659484863199</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F4" s="13">
+        <v>95.597888584822797</v>
+      </c>
+      <c r="G4" s="13">
+        <v>98.369870713884197</v>
+      </c>
+      <c r="H4" s="13">
+        <v>98.369870713884197</v>
+      </c>
+      <c r="I4" s="1">
+        <v>98.763350196739694</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>0.98819561551433399</v>
       </c>
@@ -1157,11 +1430,23 @@
       <c r="C5" s="1">
         <v>3.5905838012695302E-4</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="1">
         <v>0.14333224296569799</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F5" s="13">
+        <v>95.595730487602395</v>
+      </c>
+      <c r="G5" s="13">
+        <v>98.426082068577799</v>
+      </c>
+      <c r="H5" s="13">
+        <v>98.313659359190495</v>
+      </c>
+      <c r="I5" s="1">
+        <v>99.213041034288906</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>0.98988195615514296</v>
       </c>
@@ -1171,11 +1456,23 @@
       <c r="C6" s="1">
         <v>1.9264221191406201E-4</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="1">
         <v>7.5737237930297796E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F6" s="13">
+        <v>96.012911289640996</v>
+      </c>
+      <c r="G6" s="13">
+        <v>98.9881956155143</v>
+      </c>
+      <c r="H6" s="13">
+        <v>98.707138842046007</v>
+      </c>
+      <c r="I6" s="1">
+        <v>98.931984260820599</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>0.98763350196739697</v>
       </c>
@@ -1185,11 +1482,23 @@
       <c r="C7" s="1">
         <v>2.5749206542968701E-4</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="1">
         <v>8.4540605545043904E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F7" s="13">
+        <v>95.411487157145501</v>
+      </c>
+      <c r="G7" s="13">
+        <v>98.819561551433395</v>
+      </c>
+      <c r="H7" s="13">
+        <v>98.819561551433395</v>
+      </c>
+      <c r="I7" s="1">
+        <v>98.763350196739694</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>0.98988195615514296</v>
       </c>
@@ -1199,11 +1508,23 @@
       <c r="C8" s="1">
         <v>1.8930435180664E-4</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="1">
         <v>7.9212427139282199E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F8" s="13">
+        <v>95.096607914550603</v>
+      </c>
+      <c r="G8" s="13">
+        <v>98.313659359190495</v>
+      </c>
+      <c r="H8" s="13">
+        <v>97.9763912310286</v>
+      </c>
+      <c r="I8" s="1">
+        <v>98.875772906126997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>0.98707138842046005</v>
       </c>
@@ -1213,11 +1534,23 @@
       <c r="C9" s="1">
         <v>2.6893615722656201E-4</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="1">
         <v>7.4156761169433594E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F9" s="13">
+        <v>95.608312469102799</v>
+      </c>
+      <c r="G9" s="13">
+        <v>98.763350196739694</v>
+      </c>
+      <c r="H9" s="13">
+        <v>98.538504777965102</v>
+      </c>
+      <c r="I9" s="1">
+        <v>98.594716132658803</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>0.98988195615514296</v>
       </c>
@@ -1227,11 +1560,23 @@
       <c r="C10" s="1">
         <v>2.5749206542968701E-4</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="1">
         <v>8.7489604949951102E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F10" s="13">
+        <v>95.815675474430506</v>
+      </c>
+      <c r="G10" s="13">
+        <v>98.931984260820599</v>
+      </c>
+      <c r="H10" s="13">
+        <v>98.594716132658803</v>
+      </c>
+      <c r="I10" s="1">
+        <v>98.426082068577799</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>0.98538504777965097</v>
       </c>
@@ -1241,11 +1586,23 @@
       <c r="C11" s="1">
         <v>2.5749206542968701E-4</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="1">
         <v>0.10050606727600001</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F11" s="13">
+        <v>95.918629869640398</v>
+      </c>
+      <c r="G11" s="13">
+        <v>98.763350196739694</v>
+      </c>
+      <c r="H11" s="13">
+        <v>98.707138842046007</v>
+      </c>
+      <c r="I11" s="1">
+        <v>98.707138842046007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>0.98931984260820605</v>
       </c>
@@ -1255,20 +1612,32 @@
       <c r="C12" s="1">
         <v>2.47955322265625E-4</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="1">
         <v>8.4836483001708901E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F12" s="13">
+        <v>96.243645439169995</v>
+      </c>
+      <c r="G12" s="13">
+        <v>98.707138842046007</v>
+      </c>
+      <c r="H12" s="13">
+        <v>98.538504777965102</v>
+      </c>
+      <c r="I12" s="1">
+        <v>98.4822934232715</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
@@ -1289,18 +1658,19 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82957BC5-845A-415D-A9C1-AC076A441DA7}">
-  <dimension ref="A2:D12"/>
+  <dimension ref="A2:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="I3" sqref="I3:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1309,7 +1679,7 @@
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1322,8 +1692,20 @@
       <c r="D2" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0.98819561551433399</v>
       </c>
@@ -1336,8 +1718,20 @@
       <c r="D3" s="1">
         <v>0.111749172210693</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F3" s="1">
+        <v>95.445640491070407</v>
+      </c>
+      <c r="G3" s="1">
+        <v>97.695334457560406</v>
+      </c>
+      <c r="H3" s="1">
+        <v>98.201236649803207</v>
+      </c>
+      <c r="I3" s="1">
+        <v>98.9881956155143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>0.99044406970207899</v>
       </c>
@@ -1350,8 +1744,20 @@
       <c r="D4" s="1">
         <v>0.113413095474243</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F4" s="1">
+        <v>95.527249525898</v>
+      </c>
+      <c r="G4" s="1">
+        <v>97.751545812253994</v>
+      </c>
+      <c r="H4" s="1">
+        <v>98.369870713884197</v>
+      </c>
+      <c r="I4" s="1">
+        <v>99.100618324901603</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>0.98482293423271505</v>
       </c>
@@ -1364,8 +1770,20 @@
       <c r="D5" s="1">
         <v>0.11999559402465799</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F5" s="1">
+        <v>94.849485539795097</v>
+      </c>
+      <c r="G5" s="1">
+        <v>97.920179876334998</v>
+      </c>
+      <c r="H5" s="1">
+        <v>98.538504777965102</v>
+      </c>
+      <c r="I5" s="1">
+        <v>98.763350196739694</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>0.98482293423271505</v>
       </c>
@@ -1378,8 +1796,20 @@
       <c r="D6" s="1">
         <v>0.11184048652648899</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F6" s="1">
+        <v>96.327491532189299</v>
+      </c>
+      <c r="G6" s="1">
+        <v>98.088813940415903</v>
+      </c>
+      <c r="H6" s="1">
+        <v>98.594716132658803</v>
+      </c>
+      <c r="I6" s="1">
+        <v>98.538504777965102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>0.99213041034288896</v>
       </c>
@@ -1392,8 +1822,20 @@
       <c r="D7" s="1">
         <v>0.129948616027832</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F7" s="1">
+        <v>96.173441384229207</v>
+      </c>
+      <c r="G7" s="1">
+        <v>98.369870713884197</v>
+      </c>
+      <c r="H7" s="1">
+        <v>98.707138842046007</v>
+      </c>
+      <c r="I7" s="1">
+        <v>98.594716132658803</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>0.98707138842046005</v>
       </c>
@@ -1406,8 +1848,20 @@
       <c r="D8" s="1">
         <v>0.10836601257324199</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F8" s="1">
+        <v>95.6768108328708</v>
+      </c>
+      <c r="G8" s="1">
+        <v>98.257448004496894</v>
+      </c>
+      <c r="H8" s="1">
+        <v>98.707138842046007</v>
+      </c>
+      <c r="I8" s="1">
+        <v>98.369870713884197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>0.98650927487352402</v>
       </c>
@@ -1420,8 +1874,20 @@
       <c r="D9" s="1">
         <v>0.110030174255371</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F9" s="1">
+        <v>95.189856887107098</v>
+      </c>
+      <c r="G9" s="1">
+        <v>97.920179876334998</v>
+      </c>
+      <c r="H9" s="1">
+        <v>98.4822934232715</v>
+      </c>
+      <c r="I9" s="1">
+        <v>98.9881956155143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>0.98538504777965097</v>
       </c>
@@ -1434,8 +1900,20 @@
       <c r="D10" s="1">
         <v>0.114490270614624</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F10" s="1">
+        <v>95.922736060779599</v>
+      </c>
+      <c r="G10" s="1">
+        <v>98.707138842046007</v>
+      </c>
+      <c r="H10" s="1">
+        <v>99.044406970207902</v>
+      </c>
+      <c r="I10" s="1">
+        <v>98.707138842046007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>0.98707138842046005</v>
       </c>
@@ -1448,8 +1926,20 @@
       <c r="D11" s="1">
         <v>0.117451429367065</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F11" s="1">
+        <v>95.211941951795595</v>
+      </c>
+      <c r="G11" s="1">
+        <v>97.863968521641297</v>
+      </c>
+      <c r="H11" s="1">
+        <v>98.4822934232715</v>
+      </c>
+      <c r="I11" s="1">
+        <v>98.426082068577799</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>0.98707138842046005</v>
       </c>
@@ -1462,30 +1952,46 @@
       <c r="D12" s="1">
         <v>0.119558572769165</v>
       </c>
+      <c r="F12" s="1">
+        <v>95.243722180670503</v>
+      </c>
+      <c r="G12" s="1">
+        <v>97.526700393479402</v>
+      </c>
+      <c r="H12" s="1">
+        <v>98.650927487352405</v>
+      </c>
+      <c r="I12" s="1">
+        <v>98.819561551433395</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199A48B2-ACE2-47BC-9446-650C2E182FA4}">
-  <dimension ref="A2:C12"/>
+  <dimension ref="A2:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.77734375" style="1"/>
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1496,7 +2002,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0.98819561551433399</v>
       </c>
@@ -1507,7 +2013,7 @@
         <v>7.5984001159667904E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>0.99044406970207899</v>
       </c>
@@ -1518,7 +2024,7 @@
         <v>2.1140575408935499E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>0.98707138842046005</v>
       </c>
@@ -1529,7 +2035,7 @@
         <v>6.7448616027831999E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>0.98988195615514296</v>
       </c>
@@ -1540,7 +2046,7 @@
         <v>6.7448616027831999E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>0.98707138842046005</v>
       </c>
@@ -1551,7 +2057,7 @@
         <v>1.2099742889404199E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>0.98707138842046005</v>
       </c>
@@ -1562,7 +2068,7 @@
         <v>7.5864791870117101E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>0.983698707138842</v>
       </c>
@@ -1573,7 +2079,7 @@
         <v>9.1624259948730404E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>0.98763350196739697</v>
       </c>
@@ -1584,7 +2090,7 @@
         <v>7.1120262145995996E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>0.98538504777965097</v>
       </c>
@@ -1595,7 +2101,7 @@
         <v>6.7281723022460905E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>0.985947161326588</v>
       </c>
@@ -1606,10 +2112,184 @@
         <v>1.0626316070556599E-3</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="27">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="D15" s="27">
+        <v>200.197</v>
+      </c>
+      <c r="E15" s="27">
+        <f>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</f>
+        <v>68094.217687074837</v>
+      </c>
+      <c r="F15" s="27">
+        <f t="shared" ref="F15" si="0">0.023</f>
+        <v>2.3E-2</v>
+      </c>
+      <c r="G15" s="27">
+        <v>3.9769999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="27">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="D16" s="27">
+        <v>200.197</v>
+      </c>
+      <c r="E16" s="27">
+        <f>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</f>
+        <v>68326.621160409559</v>
+      </c>
+      <c r="F16" s="27">
+        <v>2.3E-2</v>
+      </c>
+      <c r="G16" s="27">
+        <v>3.9769999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="27">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="D17" s="27">
+        <v>200.197</v>
+      </c>
+      <c r="E17" s="27">
+        <f>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</f>
+        <v>68094.217687074837</v>
+      </c>
+      <c r="F17" s="27">
+        <v>2.3E-2</v>
+      </c>
+      <c r="G17" s="27">
+        <v>3.9769999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="27">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="D18" s="27">
+        <v>200.197</v>
+      </c>
+      <c r="E18" s="27">
+        <f>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</f>
+        <v>67406.39730639731</v>
+      </c>
+      <c r="F18" s="27">
+        <v>2.3E-2</v>
+      </c>
+      <c r="G18" s="27">
+        <v>3.9769999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="27">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="D19" s="27">
+        <v>200.197</v>
+      </c>
+      <c r="E19" s="27">
+        <f>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</f>
+        <v>67863.389830508488</v>
+      </c>
+      <c r="F19" s="27">
+        <v>2.3E-2</v>
+      </c>
+      <c r="G19" s="27">
+        <v>3.9769999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="28">
+        <f>AVERAGE(C15:C19)</f>
+        <v>0.29459999999999997</v>
+      </c>
+      <c r="D20" s="28">
+        <f t="shared" ref="D20:G20" si="1">AVERAGE(D15:D19)</f>
+        <v>200.197</v>
+      </c>
+      <c r="E20" s="28">
+        <f t="shared" si="1"/>
+        <v>67956.968734293012</v>
+      </c>
+      <c r="F20" s="28">
+        <f t="shared" si="1"/>
+        <v>2.3E-2</v>
+      </c>
+      <c r="G20" s="28">
+        <f t="shared" si="1"/>
+        <v>3.9769999999999994</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adjusted filenames of dashing scripts; edited client app to try different dashing releases if necessary
</commit_message>
<xml_diff>
--- a/ML_Model_Scripts/Performance Data/New performance data.xlsx
+++ b/ML_Model_Scripts/Performance Data/New performance data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\vivs\Documents\concreteml-covid-classifier\ML_Model_Scripts\Performance Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12962A6-A4F2-4E97-83A0-83DEDEF4BD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D865F124-61AE-4BEA-A9C9-67879F77A6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,8 +19,8 @@
     <sheet name="fhe (+ sizes)" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="micromultiplier">Overall!$C$9</definedName>
-    <definedName name="unit">Overall!$B$9</definedName>
+    <definedName name="micromultiplier">Overall!$C$10</definedName>
+    <definedName name="unit">Overall!$B$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="66">
   <si>
     <t>Plaintext</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>test set size</t>
-  </si>
-  <si>
-    <t>how many times slower?</t>
   </si>
   <si>
     <t>Test Machine Specifications</t>
@@ -217,23 +214,47 @@
 (for seconds)</t>
   </si>
   <si>
-    <t>microseconds</t>
-  </si>
-  <si>
     <t>recall_score</t>
   </si>
   <si>
-    <t>recall score</t>
+    <t>sensitivity (recall_score)</t>
+  </si>
+  <si>
+    <t>Prediction is 
+how many times slower?</t>
+  </si>
+  <si>
+    <t>128-bit security required to match concrete-ml security level</t>
+  </si>
+  <si>
+    <t>Linux Compatibility Layer</t>
+  </si>
+  <si>
+    <t>Windows Subsystem for Linux 2 (using Ubuntu 22.04 LTS)</t>
+  </si>
+  <si>
+    <t>nanoseconds</t>
+  </si>
+  <si>
+    <t>run no.</t>
+  </si>
+  <si>
+    <t>compilation time in seconds</t>
+  </si>
+  <si>
+    <t>compilation time in nanoseconds</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000000%"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -458,12 +479,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -489,6 +504,24 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -498,61 +531,49 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -560,7 +581,191 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="56">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="0.0000"/>
       <fill>
@@ -578,149 +783,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -799,90 +861,103 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{394116DB-3FC4-462F-A6EA-93CE28E8DEFC}" name="Table1" displayName="Table1" ref="A2:E12" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
-  <autoFilter ref="A2:E12" xr:uid="{394116DB-3FC4-462F-A6EA-93CE28E8DEFC}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{CFED003A-DA1B-4CE5-8524-E8936E3DBC3E}" name="accuracy" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{E1948511-7D29-400B-AA26-A9E601B91AEC}" name="roc_auc_score" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{7A51BA68-3B03-403B-89BD-9395BC2871EB}" name="test_set_prediction_time" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{832497D3-116A-4DE3-A927-E67DAAF345F9}" name="training_time" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{6BF1096A-6B0A-4B1A-BD35-2A1207399D49}" name="recall_score" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E9CFD89E-23B4-4900-868A-D7C63CC3629E}" name="Table10" displayName="Table10" ref="A30:B41" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2">
+  <autoFilter ref="A30:B41" xr:uid="{E9CFD89E-23B4-4900-868A-D7C63CC3629E}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{FDD77692-0B2D-40D7-9D09-720C76DC1D39}" name="run no." dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{BE378DC4-90AA-4B9F-B636-DD04BF9D4413}" name="compilation time in nanoseconds" dataDxfId="0">
+      <calculatedColumnFormula>'fhe (+ sizes)'!F23*micromultiplier</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4BDC63FC-A3D1-4A76-971A-2D7E1A53E2E0}" name="Table5" displayName="Table5" ref="G2:J12" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
-  <autoFilter ref="G2:J12" xr:uid="{4BDC63FC-A3D1-4A76-971A-2D7E1A53E2E0}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{590571B2-7F3A-4AB4-82F6-490D3ABC5319}" name="Linear Regression" dataDxfId="40" dataCellStyle="Percent"/>
-    <tableColumn id="2" xr3:uid="{07D40D9A-323F-4837-9150-E888FA1F58E4}" name="Random Forest" dataDxfId="39" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{852582AB-50FA-439E-807C-CDA24D4C70C4}" name="SVC" dataDxfId="38" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{799C5940-B5F5-4EC3-89E0-C94AD8F231A7}" name="Logistic Regression" dataDxfId="37" dataCellStyle="Percent"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{394116DB-3FC4-462F-A6EA-93CE28E8DEFC}" name="Table1" displayName="Table1" ref="A2:E12" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+  <autoFilter ref="A2:E12" xr:uid="{394116DB-3FC4-462F-A6EA-93CE28E8DEFC}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{CFED003A-DA1B-4CE5-8524-E8936E3DBC3E}" name="accuracy" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{E1948511-7D29-400B-AA26-A9E601B91AEC}" name="roc_auc_score" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{7A51BA68-3B03-403B-89BD-9395BC2871EB}" name="test_set_prediction_time" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{832497D3-116A-4DE3-A927-E67DAAF345F9}" name="training_time" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{6BF1096A-6B0A-4B1A-BD35-2A1207399D49}" name="recall_score" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{51C47605-6D87-4135-B9CB-CCDCB9C5785B}" name="Table2" displayName="Table2" ref="A2:E12" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A2:E12" xr:uid="{51C47605-6D87-4135-B9CB-CCDCB9C5785B}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D1463535-C8C0-4CDA-8D2E-CC2600120E02}" name="accuracy" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{B5EFEA31-5244-404F-A004-FB2C24EF05C5}" name="roc_auc_score" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{4ECC1606-A197-4F05-B01C-AE05A7881542}" name="test_set_prediction_time" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{5607816E-855A-4944-AF8F-D298454F5A6B}" name="training_time" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{6C282614-58D3-469E-8D4B-11E62AD2B121}" name="recall_score" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4BDC63FC-A3D1-4A76-971A-2D7E1A53E2E0}" name="Table5" displayName="Table5" ref="G2:J12" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+  <autoFilter ref="G2:J12" xr:uid="{4BDC63FC-A3D1-4A76-971A-2D7E1A53E2E0}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{590571B2-7F3A-4AB4-82F6-490D3ABC5319}" name="Linear Regression" dataDxfId="46" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{07D40D9A-323F-4837-9150-E888FA1F58E4}" name="Random Forest" dataDxfId="45" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{852582AB-50FA-439E-807C-CDA24D4C70C4}" name="SVC" dataDxfId="44" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{799C5940-B5F5-4EC3-89E0-C94AD8F231A7}" name="Logistic Regression" dataDxfId="43" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E7F5510B-26CB-48F1-9BD1-CC49FC0D68B6}" name="Table57" displayName="Table57" ref="G2:J12" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
-  <autoFilter ref="G2:J12" xr:uid="{E7F5510B-26CB-48F1-9BD1-CC49FC0D68B6}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E9413FF7-271E-469E-BCC5-DC52D55F3A3A}" name="Linear Regression" dataDxfId="29" dataCellStyle="Percent"/>
-    <tableColumn id="2" xr3:uid="{D6DB89F1-F914-4459-8D10-40E13FB298B0}" name="Random Forest" dataDxfId="28" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{C4F7B31F-A9DC-4D0B-B72F-83D8E4B839D1}" name="SVC" dataDxfId="27" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{546CB1C7-04D1-48CD-81F4-0F71D956336F}" name="Logistic Regression" dataDxfId="26" dataCellStyle="Percent"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{51C47605-6D87-4135-B9CB-CCDCB9C5785B}" name="Table2" displayName="Table2" ref="A2:E12" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+  <autoFilter ref="A2:E12" xr:uid="{51C47605-6D87-4135-B9CB-CCDCB9C5785B}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{D1463535-C8C0-4CDA-8D2E-CC2600120E02}" name="accuracy" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{B5EFEA31-5244-404F-A004-FB2C24EF05C5}" name="roc_auc_score" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{4ECC1606-A197-4F05-B01C-AE05A7881542}" name="test_set_prediction_time" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{5607816E-855A-4944-AF8F-D298454F5A6B}" name="training_time" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{6C282614-58D3-469E-8D4B-11E62AD2B121}" name="recall_score" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{274CBF2D-66AB-4A51-A1D7-B37000717CE9}" name="Table3" displayName="Table3" ref="A2:D12" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
-  <autoFilter ref="A2:D12" xr:uid="{274CBF2D-66AB-4A51-A1D7-B37000717CE9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E7F5510B-26CB-48F1-9BD1-CC49FC0D68B6}" name="Table57" displayName="Table57" ref="G2:J12" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="G2:J12" xr:uid="{E7F5510B-26CB-48F1-9BD1-CC49FC0D68B6}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CF2700D2-A674-464D-946D-1F615B6D91A7}" name="accuracy" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{2EA8A39C-2C3A-4F0F-9292-AEF706305A49}" name="roc_auc_score" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{C2D54946-E516-44E8-911A-9CDEC9118CD9}" name="test_set_prediction_time" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{32534789-56F1-416C-9548-79FD73103C70}" name="recall_score" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{E9413FF7-271E-469E-BCC5-DC52D55F3A3A}" name="Linear Regression" dataDxfId="33" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{D6DB89F1-F914-4459-8D10-40E13FB298B0}" name="Random Forest" dataDxfId="32" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{C4F7B31F-A9DC-4D0B-B72F-83D8E4B839D1}" name="SVC" dataDxfId="31" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{546CB1C7-04D1-48CD-81F4-0F71D956336F}" name="Logistic Regression" dataDxfId="30" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E5D7C54E-16E1-4754-8032-313998CAF65E}" name="Table4" displayName="Table4" ref="A14:H20" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{274CBF2D-66AB-4A51-A1D7-B37000717CE9}" name="Table3" displayName="Table3" ref="A2:D12" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="A2:D12" xr:uid="{274CBF2D-66AB-4A51-A1D7-B37000717CE9}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{CF2700D2-A674-464D-946D-1F615B6D91A7}" name="accuracy" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{2EA8A39C-2C3A-4F0F-9292-AEF706305A49}" name="roc_auc_score" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{C2D54946-E516-44E8-911A-9CDEC9118CD9}" name="test_set_prediction_time" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{32534789-56F1-416C-9548-79FD73103C70}" name="recall_score" dataDxfId="24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E5D7C54E-16E1-4754-8032-313998CAF65E}" name="Table4" displayName="Table4" ref="A14:H20" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A14:H20" xr:uid="{E5D7C54E-16E1-4754-8032-313998CAF65E}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{E078801A-15C7-4980-8156-8BD235967CEF}" name="Run no." dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{EFC1765B-5F55-4EA2-8F83-E8A7E7C44F75}" name="Strain" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{F62F3C7A-45AD-49AC-B959-B08E20AA523B}" name="Plaintext Size (kB)" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{C782FB93-D156-4C46-B517-3AE650180077}" name="Ciphertext Size (kB)" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{F4080A86-E0E6-428D-9973-84C9B618A1A8}" name="Percentage Increase" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{E078801A-15C7-4980-8156-8BD235967CEF}" name="Run no." dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{EFC1765B-5F55-4EA2-8F83-E8A7E7C44F75}" name="Strain" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{F62F3C7A-45AD-49AC-B959-B08E20AA523B}" name="Plaintext Size (kB)" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{C782FB93-D156-4C46-B517-3AE650180077}" name="Ciphertext Size (kB)" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{F4080A86-E0E6-428D-9973-84C9B618A1A8}" name="Percentage Increase" dataDxfId="17">
       <calculatedColumnFormula>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{30A9C073-FC8D-4D3E-B3F4-A25F0535FC84}" name="Eval Key Size (kB)" dataDxfId="13">
+    <tableColumn id="5" xr3:uid="{30A9C073-FC8D-4D3E-B3F4-A25F0535FC84}" name="Eval Key Size (kB)" dataDxfId="16">
       <calculatedColumnFormula>0.023</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9EE40A62-0BC7-4513-9103-444B1C53E933}" name="Private Key Size (kB)" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{9EE40A62-0BC7-4513-9103-444B1C53E933}" name="Private Key Size (kB)" dataDxfId="15">
       <calculatedColumnFormula>(Table4[[#This Row],[Run no.]]/Table4[[#This Row],[Percentage Increase]])*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{76F80D93-0ED4-416C-92DC-DF581C4F806B}" name="Increase in size vs RSA Standard" dataDxfId="11">
+    <tableColumn id="8" xr3:uid="{76F80D93-0ED4-416C-92DC-DF581C4F806B}" name="Increase in size vs RSA Standard" dataDxfId="14">
       <calculatedColumnFormula>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -890,14 +965,25 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{921BAE21-4B96-4F12-A7A8-47BA9506F67C}" name="Table578" displayName="Table578" ref="F2:I12" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{921BAE21-4B96-4F12-A7A8-47BA9506F67C}" name="Table578" displayName="Table578" ref="F2:I12" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="F2:I12" xr:uid="{921BAE21-4B96-4F12-A7A8-47BA9506F67C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{97A1ECBF-985D-4294-89E3-45BDAA49FAAD}" name="Linear Regression" dataDxfId="8" dataCellStyle="Percent"/>
-    <tableColumn id="2" xr3:uid="{F3A1317D-74D5-4E25-BF5E-D8D4B3C2EF7B}" name="Random Forest" dataDxfId="7" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{FB9C8954-66F5-4DE2-BE3E-4A8164D0FCB3}" name="SVC" dataDxfId="6" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{907A467A-FA21-4927-B99F-EE5170044BB4}" name="Logistic Regression" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{97A1ECBF-985D-4294-89E3-45BDAA49FAAD}" name="Linear Regression" dataDxfId="11" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{F3A1317D-74D5-4E25-BF5E-D8D4B3C2EF7B}" name="Random Forest" dataDxfId="10" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{FB9C8954-66F5-4DE2-BE3E-4A8164D0FCB3}" name="SVC" dataDxfId="9" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{907A467A-FA21-4927-B99F-EE5170044BB4}" name="Logistic Regression" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{06850F0F-1F82-486C-991A-803478B128DC}" name="Table8" displayName="Table8" ref="E22:F33" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5">
+  <autoFilter ref="E22:F33" xr:uid="{06850F0F-1F82-486C-991A-803478B128DC}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{E69931A7-7281-4236-B5F1-8FA661C967FE}" name="run no." dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{8C071A2A-7EC5-49A2-87BF-5DD99FB58EDF}" name="compilation time in seconds" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1166,16 +1252,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:M27"/>
+  <dimension ref="A3:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="31.77734375" style="1" customWidth="1"/>
     <col min="5" max="5" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35.77734375" style="1" bestFit="1" customWidth="1"/>
@@ -1189,13 +1275,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="30"/>
+      <c r="A3" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="45"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="45"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -1204,474 +1290,596 @@
       <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="27" t="s">
+      <c r="D4" s="32"/>
+      <c r="E4" s="33"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="33"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="32"/>
+      <c r="E6" s="33"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="32"/>
+      <c r="E7" s="33"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="28"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="28"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="28"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+      <c r="B8" s="30"/>
+      <c r="C8" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="27" t="s">
+      <c r="D8" s="32"/>
+      <c r="E8" s="33"/>
+    </row>
+    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="4">
+        <f>IF(ISNUMBER(SEARCH("nano", unit)),1000000000, 1000000)</f>
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="28"/>
-    </row>
-    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="42"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="38" t="str">
+        <f xml:space="preserve"> "running time (" &amp; unit &amp; ")"</f>
+        <v>running time (nanoseconds)</v>
+      </c>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="36"/>
+    </row>
+    <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="4">
-        <f>IF(ISNUMBER(SEARCH("micro", unit)), 1000000, 100000)</f>
-        <v>1000000</v>
-      </c>
-      <c r="D9" s="42"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="35" t="str">
-        <f xml:space="preserve"> "running time (" &amp; unit &amp; ")"</f>
-        <v>running time (microseconds)</v>
-      </c>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="33"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="20" t="str">
+      <c r="E15" s="18" t="str">
         <f>"entire test set (" &amp; unit &amp; ")"</f>
-        <v>entire test set (microseconds)</v>
-      </c>
-      <c r="F14" s="20" t="str">
+        <v>entire test set (nanoseconds)</v>
+      </c>
+      <c r="F15" s="18" t="str">
         <f>"average per-sample time (" &amp; unit &amp; ")"</f>
-        <v>average per-sample time (microseconds)</v>
-      </c>
-      <c r="G14" s="21" t="str">
+        <v>average per-sample time (nanoseconds)</v>
+      </c>
+      <c r="G15" s="19" t="str">
         <f>"training time (" &amp; unit &amp; ")"</f>
-        <v>training time (microseconds)</v>
-      </c>
-      <c r="H14" s="21" t="str">
+        <v>training time (nanoseconds)</v>
+      </c>
+      <c r="H15" s="19" t="str">
         <f>"quantization time (" &amp; unit &amp; ")"</f>
-        <v>quantization time (microseconds)</v>
-      </c>
-      <c r="I14" s="22" t="s">
+        <v>quantization time (nanoseconds)</v>
+      </c>
+      <c r="I15" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="J14" s="22" t="s">
+      <c r="J15" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K14" s="22" t="s">
+      <c r="K15" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="L15" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="L14" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="M14" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
+      <c r="M15" s="28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B16" s="25">
         <f>AVERAGE('scikit-learn'!A3:A21)</f>
         <v>0.98830803822372082</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C16" s="27">
         <f>AVERAGE('scikit-learn'!B3:B12)</f>
         <v>0.99658827633862868</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D16" s="25">
         <f>AVERAGE(Table1[recall_score])/100</f>
         <v>0.98746479999999992</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E16" s="27">
         <f>AVERAGE(Table1[test_set_prediction_time])*micromultiplier</f>
-        <v>267.0526504516597</v>
-      </c>
-      <c r="F15" s="14">
-        <f>E15/$A$20</f>
-        <v>0.15011391256417073</v>
-      </c>
-      <c r="G15" s="14">
+        <v>267052.65045165969</v>
+      </c>
+      <c r="F16" s="27">
+        <f>E16/$A$21</f>
+        <v>150.1139125641707</v>
+      </c>
+      <c r="G16" s="27">
         <f>AVERAGE(Table1[training_time])*micromultiplier</f>
-        <v>95986.247062682844</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" s="16">
-        <f>ABS(B15-$B$15)</f>
+        <v>95986247.062682837</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="26">
+        <f>ABS(B16-$B$16)</f>
         <v>0</v>
       </c>
-      <c r="J15" s="16">
-        <f>ABS(1-C15/$C$15)</f>
+      <c r="J16" s="26">
+        <f>ABS(1-C16/$C$16)</f>
         <v>0</v>
       </c>
-      <c r="K15" s="16">
-        <f>ABS(1-E15/$E$15)</f>
+      <c r="K16" s="26">
+        <f>ABS(1-E16/$E$16)</f>
         <v>0</v>
       </c>
-      <c r="L15" s="16">
-        <f>ABS(1-(G15/$G$15))</f>
+      <c r="L16" s="26">
+        <f>ABS(1-(G16/$G$16))</f>
         <v>0</v>
       </c>
-      <c r="M15" s="16" t="str">
-        <f xml:space="preserve"> ROUND((K15),2) &amp; "x slower"</f>
+      <c r="M16" s="14" t="str">
+        <f xml:space="preserve"> ROUND((K16),2) &amp; "x slower"</f>
         <v>0x slower</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="19" t="s">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B17" s="25">
         <f>AVERAGE('quantized plaintext'!A3:A12)</f>
         <v>0.98735244519392873</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C17" s="27">
         <f>AVERAGE('quantized plaintext'!B3:B12)</f>
         <v>0.99657517421600195</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D17" s="25">
         <f>AVERAGE(Table2[recall_score])/100</f>
         <v>0.98656560000000015</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E17" s="27">
         <f>AVERAGE(Table2[test_set_prediction_time])*micromultiplier</f>
-        <v>819.32544708251748</v>
-      </c>
-      <c r="F16" s="14">
-        <f t="shared" ref="F16:F17" si="0">E16/$A$20</f>
-        <v>0.46055393315487209</v>
-      </c>
-      <c r="G16" s="14">
+        <v>819325.44708251744</v>
+      </c>
+      <c r="F17" s="27">
+        <f t="shared" ref="F17:F18" si="0">E17/$A$21</f>
+        <v>460.55393315487208</v>
+      </c>
+      <c r="G17" s="27">
         <f>AVERAGE(Table2[training_time])*micromultiplier</f>
-        <v>115684.34238433819</v>
-      </c>
-      <c r="H16" s="14">
-        <f>G16-$G$15</f>
-        <v>19698.095321655346</v>
-      </c>
-      <c r="I16" s="16">
-        <f>ABS(B16-$B$15)</f>
+        <v>115684342.3843382</v>
+      </c>
+      <c r="H17" s="27">
+        <f>G17-$G$16</f>
+        <v>19698095.321655363</v>
+      </c>
+      <c r="I17" s="26">
+        <f>ABS(B17-$B$16)</f>
         <v>9.5559302979209004E-4</v>
       </c>
-      <c r="J16" s="16">
-        <f>ABS(1-C16/$C$15)</f>
+      <c r="J17" s="26">
+        <f>ABS(1-C17/$C$16)</f>
         <v>1.3146976477473871E-5</v>
       </c>
-      <c r="K16" s="16">
-        <f>ABS(1-E16/$E$15)</f>
+      <c r="K17" s="26">
+        <f>ABS(1-E17/$E$16)</f>
         <v>2.068029640210693</v>
       </c>
-      <c r="L16" s="16">
-        <f>ABS(1-(G16/$G$15))</f>
-        <v>0.20521789240068644</v>
-      </c>
-      <c r="M16" s="16" t="str">
-        <f t="shared" ref="M16:M17" si="1" xml:space="preserve"> ROUND((K16),2) &amp; "x slower"</f>
+      <c r="L17" s="26">
+        <f>ABS(1-(G17/$G$16))</f>
+        <v>0.20521789240068666</v>
+      </c>
+      <c r="M17" s="14" t="str">
+        <f t="shared" ref="M17:M18" si="1" xml:space="preserve"> ROUND((K17),2) &amp; "x slower"</f>
         <v>2.07x slower</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="19" t="s">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B18" s="25">
         <f>AVERAGE('fhe (+ sizes)'!A3:A12)</f>
         <v>0.98724002248454146</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C18" s="27">
         <f>AVERAGE('fhe (+ sizes)'!B3:B12)</f>
         <v>0.9965799561046621</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D18" s="25">
         <f>AVERAGE(Table3[recall_score])/100</f>
         <v>0.98594709999999997</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E18" s="27">
         <f>AVERAGE(Table3[test_set_prediction_time])*micromultiplier</f>
-        <v>955.43861389159929</v>
-      </c>
-      <c r="F17" s="14">
+        <v>955438.61389159935</v>
+      </c>
+      <c r="F18" s="27">
         <f t="shared" si="0"/>
-        <v>0.53706498813468195</v>
-      </c>
-      <c r="G17" s="14">
+        <v>537.06498813468204</v>
+      </c>
+      <c r="G18" s="27">
         <f>AVERAGE(Table2[training_time])*micromultiplier</f>
-        <v>115684.34238433819</v>
-      </c>
-      <c r="H17" s="14">
-        <f>G17-$G$15</f>
-        <v>19698.095321655346</v>
-      </c>
-      <c r="I17" s="16">
-        <f>ABS(B17-$B$15)</f>
+        <v>115684342.3843382</v>
+      </c>
+      <c r="H18" s="27">
+        <f>G18-$G$16</f>
+        <v>19698095.321655363</v>
+      </c>
+      <c r="I18" s="26">
+        <f>ABS(B18-$B$16)</f>
         <v>1.0680157391793621E-3</v>
       </c>
-      <c r="J17" s="16">
-        <f>ABS(1-C17/$C$15)</f>
+      <c r="J18" s="26">
+        <f>ABS(1-C18/$C$16)</f>
         <v>8.3487174835639166E-6</v>
       </c>
-      <c r="K17" s="16">
-        <f>ABS(1-E17/$E$15)</f>
-        <v>2.5777162753325573</v>
-      </c>
-      <c r="L17" s="16">
-        <f>ABS(1-(G17/$G$15))</f>
-        <v>0.20521789240068644</v>
-      </c>
-      <c r="M17" s="16" t="str">
+      <c r="K18" s="26">
+        <f>ABS(1-E18/$E$16)</f>
+        <v>2.5777162753325578</v>
+      </c>
+      <c r="L18" s="26">
+        <f>ABS(1-(G18/$G$16))</f>
+        <v>0.20521789240068666</v>
+      </c>
+      <c r="M18" s="14" t="str">
         <f t="shared" si="1"/>
         <v>2.58x slower</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
         <v>1779</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I21" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K20" s="11" t="s">
+      <c r="L21" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="M21" s="9"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="L20" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="M20" s="9"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="J22" s="1" t="str">
+        <f>ROUND(ABS(1-(E17/$E$16)),2) &amp; "x slower"</f>
+        <v>2.07x slower</v>
+      </c>
+      <c r="K22" s="1" t="str">
+        <f>ROUND(ABS(1-(F17/$F$16)),2) &amp; "x slower"</f>
+        <v>2.07x slower</v>
+      </c>
+      <c r="L22" s="1" t="str">
+        <f>ROUND(ABS(1-(G17/$G$16)),2) &amp; "x slower"</f>
+        <v>0.21x slower</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I23" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="1" t="str">
-        <f>ROUND(ABS(1-(E16/$E$15)),2) &amp; "x slower"</f>
-        <v>2.07x slower</v>
-      </c>
-      <c r="K21" s="1" t="str">
-        <f>ROUND(ABS(1-(F16/$F$15)),2) &amp; "x slower"</f>
-        <v>2.07x slower</v>
-      </c>
-      <c r="L21" s="1" t="str">
-        <f>ROUND(ABS(1-(G16/$G$15)),2) &amp; "x slower"</f>
+      <c r="J23" s="1" t="str">
+        <f>ROUND(ABS(1-(E18/$E$16)),2) &amp; "x slower"</f>
+        <v>2.58x slower</v>
+      </c>
+      <c r="K23" s="1" t="str">
+        <f>ROUND(ABS(1-(F18/$F$16)),2) &amp; "x slower"</f>
+        <v>2.58x slower</v>
+      </c>
+      <c r="L23" s="1" t="str">
+        <f>ROUND(ABS(1-(G18/$G$16)),2) &amp; "x slower"</f>
         <v>0.21x slower</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I22" s="10" t="s">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I24" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="J22" s="1" t="str">
-        <f>ROUND(ABS(1-(E17/$E$15)),2) &amp; "x slower"</f>
-        <v>2.58x slower</v>
-      </c>
-      <c r="K22" s="1" t="str">
-        <f>ROUND(ABS(1-(F17/$F$15)),2) &amp; "x slower"</f>
-        <v>2.58x slower</v>
-      </c>
-      <c r="L22" s="1" t="str">
-        <f>ROUND(ABS(1-(G17/$G$15)),2) &amp; "x slower"</f>
-        <v>0.21x slower</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I23" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="J23" s="1" t="str">
-        <f>ROUND(ABS(1-(E17/$E$16)),2) &amp; "x slower"</f>
+      <c r="J24" s="1" t="str">
+        <f>ROUND(ABS(1-(E18/$E$17)),2) &amp; "x slower"</f>
         <v>0.17x slower</v>
       </c>
-      <c r="K23" s="1" t="str">
-        <f>ROUND(ABS(1-(F17/$F$16)),2) &amp; "x slower"</f>
+      <c r="K24" s="1" t="str">
+        <f>ROUND(ABS(1-(F18/$F$17)),2) &amp; "x slower"</f>
         <v>0.17x slower</v>
       </c>
-      <c r="L23" s="1" t="str">
-        <f>ROUND(ABS(1-(G17/$G$16)),2) &amp; "x slower"</f>
+      <c r="L24" s="1" t="str">
+        <f>ROUND(ABS(1-(G18/$G$17)),2) &amp; "x slower"</f>
         <v>0x slower</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B26" s="25">
         <f>AVERAGE(Table5[Linear Regression])</f>
         <v>0.95924138668155945</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C26" s="25">
         <f>AVERAGE(Table5[Random Forest])</f>
         <v>0.9871275997751543</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D26" s="25">
         <f>AVERAGE(Table5[SVC])</f>
         <v>0.98499156829679568</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E26" s="25">
         <f>AVERAGE(Table5[Logistic Regression])</f>
         <v>0.98802698145025247</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B27" s="25">
         <f>AVERAGE(Table57[Linear Regression])</f>
         <v>0.95945015062941796</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C27" s="25">
         <f>AVERAGE(Table57[Random Forest])</f>
         <v>0.98038223721191642</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D27" s="25">
         <f>AVERAGE(Table57[SVC])</f>
         <v>0.98566610455311943</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E27" s="25">
         <f>AVERAGE(Table57[Logistic Regression])</f>
         <v>0.98560989319842562</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B28" s="25">
         <f>AVERAGE(Table578[Linear Regression])</f>
         <v>0.95795991505585998</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C28" s="25">
         <f>AVERAGE(Table578[Random Forest])</f>
         <v>0.98116919617762766</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D28" s="25">
         <f>AVERAGE(Table578[SVC])</f>
         <v>0.98555368184373204</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E28" s="25">
         <f>AVERAGE(Table578[Logistic Regression])</f>
         <v>0.98718381112984799</v>
       </c>
     </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1">
+        <f>'fhe (+ sizes)'!F23*micromultiplier</f>
+        <v>2047241449.3560703</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>2</v>
+      </c>
+      <c r="B32" s="1">
+        <f>'fhe (+ sizes)'!F24*micromultiplier</f>
+        <v>2026603460.3118799</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>3</v>
+      </c>
+      <c r="B33" s="1">
+        <f>'fhe (+ sizes)'!F25*micromultiplier</f>
+        <v>1970088005.0659099</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1">
+        <f>'fhe (+ sizes)'!F26*micromultiplier</f>
+        <v>2024210453.0334401</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>5</v>
+      </c>
+      <c r="B35" s="1">
+        <f>'fhe (+ sizes)'!F27*micromultiplier</f>
+        <v>1939769744.87304</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>6</v>
+      </c>
+      <c r="B36" s="1">
+        <f>'fhe (+ sizes)'!F28*micromultiplier</f>
+        <v>2018125772.4761901</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>7</v>
+      </c>
+      <c r="B37" s="1">
+        <f>'fhe (+ sizes)'!F29*micromultiplier</f>
+        <v>2008958339.69116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>8</v>
+      </c>
+      <c r="B38" s="1">
+        <f>'fhe (+ sizes)'!F30*micromultiplier</f>
+        <v>2048562288.2843001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>9</v>
+      </c>
+      <c r="B39" s="1">
+        <f>'fhe (+ sizes)'!F31*micromultiplier</f>
+        <v>2002124786.37695</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>10</v>
+      </c>
+      <c r="B40" s="1">
+        <f>'fhe (+ sizes)'!F32*micromultiplier</f>
+        <v>1998833179.47387</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="1">
+        <f>'fhe (+ sizes)'!F33*micromultiplier</f>
+        <v>2008451747.8942811</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="16">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:E6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:E7"/>
-    <mergeCell ref="I13:M13"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="I14:M14"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="B14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1701,22 +1909,22 @@
         <v>10</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="38" t="s">
-        <v>58</v>
+        <v>25</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1732,7 +1940,7 @@
       <c r="D3" s="1">
         <v>0.117744445800781</v>
       </c>
-      <c r="E3" s="39">
+      <c r="E3" s="23">
         <v>98.594700000000003</v>
       </c>
       <c r="G3" s="13">
@@ -1761,7 +1969,7 @@
       <c r="D4" s="1">
         <v>0.11230659484863199</v>
       </c>
-      <c r="E4" s="39">
+      <c r="E4" s="23">
         <v>98.932000000000002</v>
       </c>
       <c r="G4" s="13">
@@ -1790,7 +1998,7 @@
       <c r="D5" s="1">
         <v>0.14333224296569799</v>
       </c>
-      <c r="E5" s="39">
+      <c r="E5" s="23">
         <v>98.707099999999997</v>
       </c>
       <c r="G5" s="13">
@@ -1819,7 +2027,7 @@
       <c r="D6" s="1">
         <v>7.5737237930297796E-2</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="23">
         <v>98.650899999999993</v>
       </c>
       <c r="G6" s="13">
@@ -1848,7 +2056,7 @@
       <c r="D7" s="1">
         <v>8.4540605545043904E-2</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="23">
         <v>98.594700000000003</v>
       </c>
       <c r="G7" s="13">
@@ -1877,7 +2085,7 @@
       <c r="D8" s="1">
         <v>7.9212427139282199E-2</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="23">
         <v>98.707099999999997</v>
       </c>
       <c r="G8" s="13">
@@ -1906,7 +2114,7 @@
       <c r="D9" s="1">
         <v>7.4156761169433594E-2</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="23">
         <v>98.875799999999998</v>
       </c>
       <c r="G9" s="13">
@@ -1935,7 +2143,7 @@
       <c r="D10" s="1">
         <v>8.7489604949951102E-2</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="23">
         <v>98.875799999999998</v>
       </c>
       <c r="G10" s="13">
@@ -1964,7 +2172,7 @@
       <c r="D11" s="1">
         <v>0.10050606727600001</v>
       </c>
-      <c r="E11" s="39">
+      <c r="E11" s="23">
         <v>98.875799999999998</v>
       </c>
       <c r="G11" s="13">
@@ -1993,7 +2201,7 @@
       <c r="D12" s="1">
         <v>8.4836483001708901E-2</v>
       </c>
-      <c r="E12" s="39">
+      <c r="E12" s="23">
         <v>98.650899999999993</v>
       </c>
       <c r="G12" s="13">
@@ -2072,22 +2280,22 @@
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="38" t="s">
-        <v>58</v>
+        <v>25</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -2103,7 +2311,7 @@
       <c r="D3" s="1">
         <v>0.111749172210693</v>
       </c>
-      <c r="E3" s="39">
+      <c r="E3" s="23">
         <v>98.932000000000002</v>
       </c>
       <c r="G3" s="13">
@@ -2132,7 +2340,7 @@
       <c r="D4" s="1">
         <v>0.113413095474243</v>
       </c>
-      <c r="E4" s="39">
+      <c r="E4" s="23">
         <v>99.044399999999996</v>
       </c>
       <c r="G4" s="13">
@@ -2161,7 +2369,7 @@
       <c r="D5" s="1">
         <v>0.11999559402465799</v>
       </c>
-      <c r="E5" s="39">
+      <c r="E5" s="23">
         <v>98.538499999999999</v>
       </c>
       <c r="G5" s="13">
@@ -2190,7 +2398,7 @@
       <c r="D6" s="1">
         <v>0.11184048652648899</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="23">
         <v>98.369900000000001</v>
       </c>
       <c r="G6" s="13">
@@ -2219,7 +2427,7 @@
       <c r="D7" s="1">
         <v>0.129948616027832</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="23">
         <v>98.482299999999995</v>
       </c>
       <c r="G7" s="13">
@@ -2248,7 +2456,7 @@
       <c r="D8" s="1">
         <v>0.10836601257324199</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="23">
         <v>98.650899999999993</v>
       </c>
       <c r="G8" s="13">
@@ -2277,7 +2485,7 @@
       <c r="D9" s="1">
         <v>0.110030174255371</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="23">
         <v>98.763400000000004</v>
       </c>
       <c r="G9" s="13">
@@ -2306,7 +2514,7 @@
       <c r="D10" s="1">
         <v>0.114490270614624</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="23">
         <v>98.875799999999998</v>
       </c>
       <c r="G10" s="13">
@@ -2335,7 +2543,7 @@
       <c r="D11" s="1">
         <v>0.117451429367065</v>
       </c>
-      <c r="E11" s="39">
+      <c r="E11" s="23">
         <v>98.369900000000001</v>
       </c>
       <c r="G11" s="13">
@@ -2364,7 +2572,7 @@
       <c r="D12" s="1">
         <v>0.119558572769165</v>
       </c>
-      <c r="E12" s="39">
+      <c r="E12" s="23">
         <v>98.538499999999999</v>
       </c>
       <c r="G12" s="13">
@@ -2446,10 +2654,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199A48B2-ACE2-47BC-9446-650C2E182FA4}">
-  <dimension ref="A2:I23"/>
+  <dimension ref="A2:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2458,7 +2666,7 @@
     <col min="2" max="3" width="45.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" customWidth="1"/>
     <col min="8" max="8" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2473,19 +2681,19 @@
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2750,28 +2958,28 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="H14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -2779,7 +2987,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="7">
         <v>0.29399999999999998</v>
@@ -2800,7 +3008,7 @@
       </c>
       <c r="H15" s="2">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
-        <v>14.625</v>
+        <v>9.4166666666666661</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -2808,7 +3016,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="7">
         <v>0.29299999999999998</v>
@@ -2828,7 +3036,7 @@
       </c>
       <c r="H16" s="2">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
-        <v>14.625</v>
+        <v>9.4166666666666661</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -2836,7 +3044,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="7">
         <v>0.29399999999999998</v>
@@ -2856,7 +3064,7 @@
       </c>
       <c r="H17" s="2">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
-        <v>14.625</v>
+        <v>9.4166666666666661</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -2864,7 +3072,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="7">
         <v>0.29699999999999999</v>
@@ -2884,7 +3092,7 @@
       </c>
       <c r="H18" s="2">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
-        <v>14.625</v>
+        <v>9.4166666666666661</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -2892,7 +3100,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="7">
         <v>0.29499999999999998</v>
@@ -2912,15 +3120,15 @@
       </c>
       <c r="H19" s="2">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
-        <v>14.625</v>
+        <v>9.4166666666666661</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="C20" s="8">
         <f>AVERAGE(C15:C19)</f>
@@ -2944,33 +3152,130 @@
       </c>
       <c r="H20" s="2">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
-        <v>14.625</v>
+        <v>9.4166666666666661</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="17" t="s">
+      <c r="B22" s="15" t="s">
         <v>53</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
-        <v>2048</v>
-      </c>
-      <c r="C23" s="18">
+        <v>3072</v>
+      </c>
+      <c r="C23" s="16">
         <f>B23/8000</f>
-        <v>0.25600000000000001</v>
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2.0472414493560702</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2.0266034603118799</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E25" s="1">
+        <v>3</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1.97008800506591</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E26" s="1">
+        <v>4</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2.0242104530334402</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E27" s="1">
+        <v>5</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1.93976974487304</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E28" s="1">
+        <v>6</v>
+      </c>
+      <c r="F28" s="1">
+        <v>2.0181257724761901</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E29" s="1">
+        <v>7</v>
+      </c>
+      <c r="F29" s="1">
+        <v>2.0089583396911599</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E30" s="1">
+        <v>8</v>
+      </c>
+      <c r="F30" s="1">
+        <v>2.0485622882843</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E31" s="1">
+        <v>9</v>
+      </c>
+      <c r="F31" s="1">
+        <v>2.00212478637695</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E32" s="1">
+        <v>10</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1.9988331794738701</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F33" s="1">
+        <f>AVERAGE(F23:F32)</f>
+        <v>2.0084517478942812</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edited model scripts to save the classes to 'classes.npy' and stored classes.npy at compiled model and clientdownloads folder
</commit_message>
<xml_diff>
--- a/ML_Model_Scripts/Performance Data/New performance data.xlsx
+++ b/ML_Model_Scripts/Performance Data/New performance data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\vivs\Documents\concreteml-covid-classifier\ML_Model_Scripts\Performance Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D865F124-61AE-4BEA-A9C9-67879F77A6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D8EB2B-4142-4A85-B793-E794BF515326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
   <si>
     <t>Plaintext</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>Ciphertext Size (kB)</t>
-  </si>
-  <si>
-    <t>Percentage Increase</t>
   </si>
   <si>
     <t>Eval Key Size (kB)</t>
@@ -243,6 +240,15 @@
   </si>
   <si>
     <t>compilation time in nanoseconds</t>
+  </si>
+  <si>
+    <t>RSA Ciphertext Size (in kB)</t>
+  </si>
+  <si>
+    <t>Percentage Increase vs Plaintext2</t>
+  </si>
+  <si>
+    <t>Percentage Increase vs RSA Ciphertext</t>
   </si>
 </sst>
 </file>
@@ -581,9 +587,13 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="56">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+  <dxfs count="57">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -618,15 +628,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -642,10 +643,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -847,6 +844,19 @@
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -861,12 +871,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E9CFD89E-23B4-4900-868A-D7C63CC3629E}" name="Table10" displayName="Table10" ref="A30:B41" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E9CFD89E-23B4-4900-868A-D7C63CC3629E}" name="Table10" displayName="Table10" ref="A30:B41" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
   <autoFilter ref="A30:B41" xr:uid="{E9CFD89E-23B4-4900-868A-D7C63CC3629E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FDD77692-0B2D-40D7-9D09-720C76DC1D39}" name="run no." dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{BE378DC4-90AA-4B9F-B636-DD04BF9D4413}" name="compilation time in nanoseconds" dataDxfId="0">
-      <calculatedColumnFormula>'fhe (+ sizes)'!F23*micromultiplier</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{FDD77692-0B2D-40D7-9D09-720C76DC1D39}" name="run no." dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{BE378DC4-90AA-4B9F-B636-DD04BF9D4413}" name="compilation time in nanoseconds" dataDxfId="53">
+      <calculatedColumnFormula>'fhe (+ sizes)'!G23*micromultiplier</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -874,90 +884,93 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{394116DB-3FC4-462F-A6EA-93CE28E8DEFC}" name="Table1" displayName="Table1" ref="A2:E12" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{394116DB-3FC4-462F-A6EA-93CE28E8DEFC}" name="Table1" displayName="Table1" ref="A2:E12" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="A2:E12" xr:uid="{394116DB-3FC4-462F-A6EA-93CE28E8DEFC}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{CFED003A-DA1B-4CE5-8524-E8936E3DBC3E}" name="accuracy" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{E1948511-7D29-400B-AA26-A9E601B91AEC}" name="roc_auc_score" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{7A51BA68-3B03-403B-89BD-9395BC2871EB}" name="test_set_prediction_time" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{832497D3-116A-4DE3-A927-E67DAAF345F9}" name="training_time" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{6BF1096A-6B0A-4B1A-BD35-2A1207399D49}" name="recall_score" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{CFED003A-DA1B-4CE5-8524-E8936E3DBC3E}" name="accuracy" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{E1948511-7D29-400B-AA26-A9E601B91AEC}" name="roc_auc_score" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{7A51BA68-3B03-403B-89BD-9395BC2871EB}" name="test_set_prediction_time" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{832497D3-116A-4DE3-A927-E67DAAF345F9}" name="training_time" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{6BF1096A-6B0A-4B1A-BD35-2A1207399D49}" name="recall_score" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4BDC63FC-A3D1-4A76-971A-2D7E1A53E2E0}" name="Table5" displayName="Table5" ref="G2:J12" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4BDC63FC-A3D1-4A76-971A-2D7E1A53E2E0}" name="Table5" displayName="Table5" ref="G2:J12" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
   <autoFilter ref="G2:J12" xr:uid="{4BDC63FC-A3D1-4A76-971A-2D7E1A53E2E0}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{590571B2-7F3A-4AB4-82F6-490D3ABC5319}" name="Linear Regression" dataDxfId="46" dataCellStyle="Percent"/>
-    <tableColumn id="2" xr3:uid="{07D40D9A-323F-4837-9150-E888FA1F58E4}" name="Random Forest" dataDxfId="45" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{852582AB-50FA-439E-807C-CDA24D4C70C4}" name="SVC" dataDxfId="44" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{799C5940-B5F5-4EC3-89E0-C94AD8F231A7}" name="Logistic Regression" dataDxfId="43" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{590571B2-7F3A-4AB4-82F6-490D3ABC5319}" name="Linear Regression" dataDxfId="43" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{07D40D9A-323F-4837-9150-E888FA1F58E4}" name="Random Forest" dataDxfId="42" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{852582AB-50FA-439E-807C-CDA24D4C70C4}" name="SVC" dataDxfId="41" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{799C5940-B5F5-4EC3-89E0-C94AD8F231A7}" name="Logistic Regression" dataDxfId="40" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{51C47605-6D87-4135-B9CB-CCDCB9C5785B}" name="Table2" displayName="Table2" ref="A2:E12" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{51C47605-6D87-4135-B9CB-CCDCB9C5785B}" name="Table2" displayName="Table2" ref="A2:E12" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A2:E12" xr:uid="{51C47605-6D87-4135-B9CB-CCDCB9C5785B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D1463535-C8C0-4CDA-8D2E-CC2600120E02}" name="accuracy" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{B5EFEA31-5244-404F-A004-FB2C24EF05C5}" name="roc_auc_score" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{4ECC1606-A197-4F05-B01C-AE05A7881542}" name="test_set_prediction_time" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{5607816E-855A-4944-AF8F-D298454F5A6B}" name="training_time" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{6C282614-58D3-469E-8D4B-11E62AD2B121}" name="recall_score" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{D1463535-C8C0-4CDA-8D2E-CC2600120E02}" name="accuracy" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{B5EFEA31-5244-404F-A004-FB2C24EF05C5}" name="roc_auc_score" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{4ECC1606-A197-4F05-B01C-AE05A7881542}" name="test_set_prediction_time" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{5607816E-855A-4944-AF8F-D298454F5A6B}" name="training_time" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{6C282614-58D3-469E-8D4B-11E62AD2B121}" name="recall_score" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E7F5510B-26CB-48F1-9BD1-CC49FC0D68B6}" name="Table57" displayName="Table57" ref="G2:J12" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E7F5510B-26CB-48F1-9BD1-CC49FC0D68B6}" name="Table57" displayName="Table57" ref="G2:J12" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="G2:J12" xr:uid="{E7F5510B-26CB-48F1-9BD1-CC49FC0D68B6}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E9413FF7-271E-469E-BCC5-DC52D55F3A3A}" name="Linear Regression" dataDxfId="33" dataCellStyle="Percent"/>
-    <tableColumn id="2" xr3:uid="{D6DB89F1-F914-4459-8D10-40E13FB298B0}" name="Random Forest" dataDxfId="32" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{C4F7B31F-A9DC-4D0B-B72F-83D8E4B839D1}" name="SVC" dataDxfId="31" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{546CB1C7-04D1-48CD-81F4-0F71D956336F}" name="Logistic Regression" dataDxfId="30" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{E9413FF7-271E-469E-BCC5-DC52D55F3A3A}" name="Linear Regression" dataDxfId="30" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{D6DB89F1-F914-4459-8D10-40E13FB298B0}" name="Random Forest" dataDxfId="29" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{C4F7B31F-A9DC-4D0B-B72F-83D8E4B839D1}" name="SVC" dataDxfId="28" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{546CB1C7-04D1-48CD-81F4-0F71D956336F}" name="Logistic Regression" dataDxfId="27" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{274CBF2D-66AB-4A51-A1D7-B37000717CE9}" name="Table3" displayName="Table3" ref="A2:D12" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{274CBF2D-66AB-4A51-A1D7-B37000717CE9}" name="Table3" displayName="Table3" ref="A2:D12" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A2:D12" xr:uid="{274CBF2D-66AB-4A51-A1D7-B37000717CE9}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CF2700D2-A674-464D-946D-1F615B6D91A7}" name="accuracy" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{2EA8A39C-2C3A-4F0F-9292-AEF706305A49}" name="roc_auc_score" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{C2D54946-E516-44E8-911A-9CDEC9118CD9}" name="test_set_prediction_time" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{32534789-56F1-416C-9548-79FD73103C70}" name="recall_score" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{CF2700D2-A674-464D-946D-1F615B6D91A7}" name="accuracy" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{2EA8A39C-2C3A-4F0F-9292-AEF706305A49}" name="roc_auc_score" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{C2D54946-E516-44E8-911A-9CDEC9118CD9}" name="test_set_prediction_time" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{32534789-56F1-416C-9548-79FD73103C70}" name="recall_score" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E5D7C54E-16E1-4754-8032-313998CAF65E}" name="Table4" displayName="Table4" ref="A14:H20" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A14:H20" xr:uid="{E5D7C54E-16E1-4754-8032-313998CAF65E}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{E078801A-15C7-4980-8156-8BD235967CEF}" name="Run no." dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{EFC1765B-5F55-4EA2-8F83-E8A7E7C44F75}" name="Strain" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{F62F3C7A-45AD-49AC-B959-B08E20AA523B}" name="Plaintext Size (kB)" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{C782FB93-D156-4C46-B517-3AE650180077}" name="Ciphertext Size (kB)" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{F4080A86-E0E6-428D-9973-84C9B618A1A8}" name="Percentage Increase" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E5D7C54E-16E1-4754-8032-313998CAF65E}" name="Table4" displayName="Table4" ref="A14:I20" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A14:I20" xr:uid="{E5D7C54E-16E1-4754-8032-313998CAF65E}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{E078801A-15C7-4980-8156-8BD235967CEF}" name="Run no." dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{EFC1765B-5F55-4EA2-8F83-E8A7E7C44F75}" name="Strain" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{F62F3C7A-45AD-49AC-B959-B08E20AA523B}" name="Plaintext Size (kB)" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{C782FB93-D156-4C46-B517-3AE650180077}" name="Ciphertext Size (kB)" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{9BA734C7-F6A6-4FCB-BB59-8D1BDD20BF6A}" name="Percentage Increase vs RSA Ciphertext" dataDxfId="0">
+      <calculatedColumnFormula>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{F4080A86-E0E6-428D-9973-84C9B618A1A8}" name="Percentage Increase vs Plaintext2" dataDxfId="1">
       <calculatedColumnFormula>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{30A9C073-FC8D-4D3E-B3F4-A25F0535FC84}" name="Eval Key Size (kB)" dataDxfId="16">
+    <tableColumn id="5" xr3:uid="{30A9C073-FC8D-4D3E-B3F4-A25F0535FC84}" name="Eval Key Size (kB)" dataDxfId="14">
       <calculatedColumnFormula>0.023</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9EE40A62-0BC7-4513-9103-444B1C53E933}" name="Private Key Size (kB)" dataDxfId="15">
-      <calculatedColumnFormula>(Table4[[#This Row],[Run no.]]/Table4[[#This Row],[Percentage Increase]])*100</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{9EE40A62-0BC7-4513-9103-444B1C53E933}" name="Private Key Size (kB)" dataDxfId="13">
+      <calculatedColumnFormula>(Table4[[#This Row],[Run no.]]/Table4[[#This Row],[Percentage Increase vs Plaintext2]])*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{76F80D93-0ED4-416C-92DC-DF581C4F806B}" name="Increase in size vs RSA Standard" dataDxfId="14">
+    <tableColumn id="8" xr3:uid="{76F80D93-0ED4-416C-92DC-DF581C4F806B}" name="Increase in size vs RSA Standard" dataDxfId="12">
       <calculatedColumnFormula>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -966,24 +979,24 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{921BAE21-4B96-4F12-A7A8-47BA9506F67C}" name="Table578" displayName="Table578" ref="F2:I12" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{921BAE21-4B96-4F12-A7A8-47BA9506F67C}" name="Table578" displayName="Table578" ref="F2:I12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="F2:I12" xr:uid="{921BAE21-4B96-4F12-A7A8-47BA9506F67C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{97A1ECBF-985D-4294-89E3-45BDAA49FAAD}" name="Linear Regression" dataDxfId="11" dataCellStyle="Percent"/>
-    <tableColumn id="2" xr3:uid="{F3A1317D-74D5-4E25-BF5E-D8D4B3C2EF7B}" name="Random Forest" dataDxfId="10" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{FB9C8954-66F5-4DE2-BE3E-4A8164D0FCB3}" name="SVC" dataDxfId="9" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{907A467A-FA21-4927-B99F-EE5170044BB4}" name="Logistic Regression" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{97A1ECBF-985D-4294-89E3-45BDAA49FAAD}" name="Linear Regression" dataDxfId="9" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{F3A1317D-74D5-4E25-BF5E-D8D4B3C2EF7B}" name="Random Forest" dataDxfId="8" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{FB9C8954-66F5-4DE2-BE3E-4A8164D0FCB3}" name="SVC" dataDxfId="7" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{907A467A-FA21-4927-B99F-EE5170044BB4}" name="Logistic Regression" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{06850F0F-1F82-486C-991A-803478B128DC}" name="Table8" displayName="Table8" ref="E22:F33" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5">
-  <autoFilter ref="E22:F33" xr:uid="{06850F0F-1F82-486C-991A-803478B128DC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{06850F0F-1F82-486C-991A-803478B128DC}" name="Table8" displayName="Table8" ref="F22:G33" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="F22:G33" xr:uid="{06850F0F-1F82-486C-991A-803478B128DC}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E69931A7-7281-4236-B5F1-8FA661C967FE}" name="run no." dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{8C071A2A-7EC5-49A2-87BF-5DD99FB58EDF}" name="compilation time in seconds" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{E69931A7-7281-4236-B5F1-8FA661C967FE}" name="run no." dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{8C071A2A-7EC5-49A2-87BF-5DD99FB58EDF}" name="compilation time in seconds" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1254,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1302,11 +1315,11 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="30"/>
       <c r="C5" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="32"/>
       <c r="E5" s="33"/>
@@ -1346,10 +1359,10 @@
     </row>
     <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="4">
         <f>IF(ISNUMBER(SEARCH("nano", unit)),1000000000, 1000000)</f>
@@ -1397,7 +1410,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15" s="18" t="str">
         <f>"entire test set (" &amp; unit &amp; ")"</f>
@@ -1422,13 +1435,13 @@
         <v>9</v>
       </c>
       <c r="K15" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="L15" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="L15" s="20" t="s">
-        <v>50</v>
-      </c>
       <c r="M15" s="28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -1460,7 +1473,7 @@
         <v>95986247.062682837</v>
       </c>
       <c r="H16" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I16" s="26">
         <f>ABS(B16-$B$16)</f>
@@ -1599,16 +1612,16 @@
         <v>1779</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>11</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L21" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M21" s="9"/>
     </row>
@@ -1617,7 +1630,7 @@
         <v>23</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J22" s="1" t="str">
         <f>ROUND(ABS(1-(E17/$E$16)),2) &amp; "x slower"</f>
@@ -1637,7 +1650,7 @@
         <v>24</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J23" s="1" t="str">
         <f>ROUND(ABS(1-(E18/$E$16)),2) &amp; "x slower"</f>
@@ -1654,7 +1667,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I24" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J24" s="1" t="str">
         <f>ROUND(ABS(1-(E18/$E$17)),2) &amp; "x slower"</f>
@@ -1751,10 +1764,10 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -1762,7 +1775,7 @@
         <v>1</v>
       </c>
       <c r="B31" s="1">
-        <f>'fhe (+ sizes)'!F23*micromultiplier</f>
+        <f>'fhe (+ sizes)'!G23*micromultiplier</f>
         <v>2047241449.3560703</v>
       </c>
     </row>
@@ -1771,7 +1784,7 @@
         <v>2</v>
       </c>
       <c r="B32" s="1">
-        <f>'fhe (+ sizes)'!F24*micromultiplier</f>
+        <f>'fhe (+ sizes)'!G24*micromultiplier</f>
         <v>2026603460.3118799</v>
       </c>
     </row>
@@ -1780,7 +1793,7 @@
         <v>3</v>
       </c>
       <c r="B33" s="1">
-        <f>'fhe (+ sizes)'!F25*micromultiplier</f>
+        <f>'fhe (+ sizes)'!G25*micromultiplier</f>
         <v>1970088005.0659099</v>
       </c>
     </row>
@@ -1789,7 +1802,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1">
-        <f>'fhe (+ sizes)'!F26*micromultiplier</f>
+        <f>'fhe (+ sizes)'!G26*micromultiplier</f>
         <v>2024210453.0334401</v>
       </c>
     </row>
@@ -1798,7 +1811,7 @@
         <v>5</v>
       </c>
       <c r="B35" s="1">
-        <f>'fhe (+ sizes)'!F27*micromultiplier</f>
+        <f>'fhe (+ sizes)'!G27*micromultiplier</f>
         <v>1939769744.87304</v>
       </c>
     </row>
@@ -1807,7 +1820,7 @@
         <v>6</v>
       </c>
       <c r="B36" s="1">
-        <f>'fhe (+ sizes)'!F28*micromultiplier</f>
+        <f>'fhe (+ sizes)'!G28*micromultiplier</f>
         <v>2018125772.4761901</v>
       </c>
     </row>
@@ -1816,7 +1829,7 @@
         <v>7</v>
       </c>
       <c r="B37" s="1">
-        <f>'fhe (+ sizes)'!F29*micromultiplier</f>
+        <f>'fhe (+ sizes)'!G29*micromultiplier</f>
         <v>2008958339.69116</v>
       </c>
     </row>
@@ -1825,7 +1838,7 @@
         <v>8</v>
       </c>
       <c r="B38" s="1">
-        <f>'fhe (+ sizes)'!F30*micromultiplier</f>
+        <f>'fhe (+ sizes)'!G30*micromultiplier</f>
         <v>2048562288.2843001</v>
       </c>
     </row>
@@ -1834,7 +1847,7 @@
         <v>9</v>
       </c>
       <c r="B39" s="1">
-        <f>'fhe (+ sizes)'!F31*micromultiplier</f>
+        <f>'fhe (+ sizes)'!G31*micromultiplier</f>
         <v>2002124786.37695</v>
       </c>
     </row>
@@ -1843,16 +1856,16 @@
         <v>10</v>
       </c>
       <c r="B40" s="1">
-        <f>'fhe (+ sizes)'!F32*micromultiplier</f>
+        <f>'fhe (+ sizes)'!G32*micromultiplier</f>
         <v>1998833179.47387</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="1">
-        <f>'fhe (+ sizes)'!F33*micromultiplier</f>
+        <f>'fhe (+ sizes)'!G33*micromultiplier</f>
         <v>2008451747.8942811</v>
       </c>
     </row>
@@ -1912,7 +1925,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>27</v>
@@ -2283,7 +2296,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>27</v>
@@ -2656,17 +2669,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199A48B2-ACE2-47BC-9446-650C2E182FA4}">
   <dimension ref="A2:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.77734375" style="1"/>
-    <col min="2" max="3" width="45.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" customWidth="1"/>
-    <col min="6" max="6" width="26.33203125" customWidth="1"/>
+    <col min="2" max="4" width="45.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2681,7 +2693,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>27</v>
@@ -2961,7 +2973,7 @@
         <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2970,16 +2982,19 @@
         <v>33</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>54</v>
+      <c r="I14" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -2987,7 +3002,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="7">
         <v>0.29399999999999998</v>
@@ -2996,17 +3011,21 @@
         <v>200.197</v>
       </c>
       <c r="E15" s="7">
+        <f>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</f>
+        <v>532.85866666666664</v>
+      </c>
+      <c r="F15" s="7">
         <f>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</f>
         <v>68094.217687074837</v>
       </c>
-      <c r="F15" s="7">
-        <f t="shared" ref="F15" si="0">0.023</f>
+      <c r="G15" s="7">
+        <f t="shared" ref="G15" si="0">0.023</f>
         <v>2.3E-2</v>
       </c>
-      <c r="G15" s="7">
+      <c r="H15" s="7">
         <v>4</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
         <v>9.4166666666666661</v>
       </c>
@@ -3016,7 +3035,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="7">
         <v>0.29299999999999998</v>
@@ -3025,26 +3044,30 @@
         <v>200.197</v>
       </c>
       <c r="E16" s="7">
+        <f>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</f>
+        <v>532.85866666666664</v>
+      </c>
+      <c r="F16" s="7">
         <f>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</f>
         <v>68326.621160409559</v>
       </c>
-      <c r="F16" s="7">
+      <c r="G16" s="7">
         <v>2.3E-2</v>
       </c>
-      <c r="G16" s="7">
+      <c r="H16" s="7">
         <v>4</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I16" s="2">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
         <v>9.4166666666666661</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="7">
         <v>0.29399999999999998</v>
@@ -3053,26 +3076,30 @@
         <v>200.197</v>
       </c>
       <c r="E17" s="7">
+        <f>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</f>
+        <v>532.85866666666664</v>
+      </c>
+      <c r="F17" s="7">
         <f>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</f>
         <v>68094.217687074837</v>
       </c>
-      <c r="F17" s="7">
+      <c r="G17" s="7">
         <v>2.3E-2</v>
       </c>
-      <c r="G17" s="7">
+      <c r="H17" s="7">
         <v>4</v>
       </c>
-      <c r="H17" s="2">
+      <c r="I17" s="2">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
         <v>9.4166666666666661</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="7">
         <v>0.29699999999999999</v>
@@ -3081,26 +3108,30 @@
         <v>200.197</v>
       </c>
       <c r="E18" s="7">
+        <f>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</f>
+        <v>532.85866666666664</v>
+      </c>
+      <c r="F18" s="7">
         <f>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</f>
         <v>67406.39730639731</v>
       </c>
-      <c r="F18" s="7">
+      <c r="G18" s="7">
         <v>2.3E-2</v>
       </c>
-      <c r="G18" s="7">
+      <c r="H18" s="7">
         <v>4</v>
       </c>
-      <c r="H18" s="2">
+      <c r="I18" s="2">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
         <v>9.4166666666666661</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="7">
         <v>0.29499999999999998</v>
@@ -3109,67 +3140,78 @@
         <v>200.197</v>
       </c>
       <c r="E19" s="7">
+        <f>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</f>
+        <v>532.85866666666664</v>
+      </c>
+      <c r="F19" s="7">
         <f>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</f>
         <v>67863.389830508488</v>
       </c>
-      <c r="F19" s="7">
+      <c r="G19" s="7">
         <v>2.3E-2</v>
       </c>
-      <c r="G19" s="7">
+      <c r="H19" s="7">
         <v>4</v>
       </c>
-      <c r="H19" s="2">
+      <c r="I19" s="2">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
         <v>9.4166666666666661</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="C20" s="8">
         <f>AVERAGE(C15:C19)</f>
         <v>0.29459999999999997</v>
       </c>
       <c r="D20" s="8">
-        <f t="shared" ref="D20:G20" si="1">AVERAGE(D15:D19)</f>
+        <f t="shared" ref="D20:H20" si="1">AVERAGE(D15:D19)</f>
         <v>200.197</v>
       </c>
       <c r="E20" s="8">
+        <f>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</f>
+        <v>532.85866666666664</v>
+      </c>
+      <c r="F20" s="8">
         <f t="shared" si="1"/>
         <v>67956.968734293012</v>
       </c>
-      <c r="F20" s="8">
+      <c r="G20" s="8">
         <f t="shared" si="1"/>
         <v>2.3E-2</v>
       </c>
-      <c r="G20" s="8">
+      <c r="H20" s="8">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H20" s="2">
+      <c r="I20" s="2">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
         <v>9.4166666666666661</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B22" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
         <v>3072</v>
       </c>
@@ -3177,94 +3219,97 @@
         <f>B23/8000</f>
         <v>0.38400000000000001</v>
       </c>
-      <c r="E23" s="1">
+      <c r="D23" s="16">
+        <v>0.375</v>
+      </c>
+      <c r="F23" s="1">
         <v>1</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23" s="1">
         <v>2.0472414493560702</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>59</v>
-      </c>
-      <c r="E24" s="1">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F24" s="1">
         <v>2</v>
       </c>
-      <c r="F24" s="1">
+      <c r="G24" s="1">
         <v>2.0266034603118799</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E25" s="1">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="1">
         <v>3</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <v>1.97008800506591</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E26" s="1">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F26" s="1">
         <v>4</v>
       </c>
-      <c r="F26" s="1">
+      <c r="G26" s="1">
         <v>2.0242104530334402</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E27" s="1">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F27" s="1">
         <v>5</v>
       </c>
-      <c r="F27" s="1">
+      <c r="G27" s="1">
         <v>1.93976974487304</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E28" s="1">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F28" s="1">
         <v>6</v>
       </c>
-      <c r="F28" s="1">
+      <c r="G28" s="1">
         <v>2.0181257724761901</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E29" s="1">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F29" s="1">
         <v>7</v>
       </c>
-      <c r="F29" s="1">
+      <c r="G29" s="1">
         <v>2.0089583396911599</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E30" s="1">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F30" s="1">
         <v>8</v>
       </c>
-      <c r="F30" s="1">
+      <c r="G30" s="1">
         <v>2.0485622882843</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E31" s="1">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F31" s="1">
         <v>9</v>
       </c>
-      <c r="F31" s="1">
+      <c r="G31" s="1">
         <v>2.00212478637695</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E32" s="1">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F32" s="1">
         <v>10</v>
       </c>
-      <c r="F32" s="1">
+      <c r="G32" s="1">
         <v>1.9988331794738701</v>
       </c>
     </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E33" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F33" s="1">
-        <f>AVERAGE(F23:F32)</f>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F33" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G33" s="1">
+        <f>AVERAGE(G23:G32)</f>
         <v>2.0084517478942812</v>
       </c>
     </row>

</xml_diff>

<commit_message>
commit before trying to install on VM
</commit_message>
<xml_diff>
--- a/ML_Model_Scripts/Performance Data/New performance data.xlsx
+++ b/ML_Model_Scripts/Performance Data/New performance data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\vivs\Documents\concreteml-covid-classifier\ML_Model_Scripts\Performance Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D8EB2B-4142-4A85-B793-E794BF515326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8326644E-A926-4658-BD9C-EF05824DAEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -255,8 +255,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+  <numFmts count="4">
     <numFmt numFmtId="165" formatCode="0.0000%"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.000000%"/>
@@ -446,7 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -464,12 +463,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -489,9 +482,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -543,6 +533,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -573,13 +572,22 @@
     <xf numFmtId="165" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -589,11 +597,34 @@
   </cellStyles>
   <dxfs count="57">
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
+      <numFmt numFmtId="165" formatCode="0.0000%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -640,29 +671,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -955,22 +963,22 @@
   <autoFilter ref="A14:I20" xr:uid="{E5D7C54E-16E1-4754-8032-313998CAF65E}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{E078801A-15C7-4980-8156-8BD235967CEF}" name="Run no." dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{EFC1765B-5F55-4EA2-8F83-E8A7E7C44F75}" name="Strain" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{F62F3C7A-45AD-49AC-B959-B08E20AA523B}" name="Plaintext Size (kB)" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{C782FB93-D156-4C46-B517-3AE650180077}" name="Ciphertext Size (kB)" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{9BA734C7-F6A6-4FCB-BB59-8D1BDD20BF6A}" name="Percentage Increase vs RSA Ciphertext" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{EFC1765B-5F55-4EA2-8F83-E8A7E7C44F75}" name="Strain" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{F62F3C7A-45AD-49AC-B959-B08E20AA523B}" name="Plaintext Size (kB)" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{C782FB93-D156-4C46-B517-3AE650180077}" name="Ciphertext Size (kB)" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{9BA734C7-F6A6-4FCB-BB59-8D1BDD20BF6A}" name="Percentage Increase vs RSA Ciphertext" dataDxfId="4" dataCellStyle="Percent">
       <calculatedColumnFormula>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F4080A86-E0E6-428D-9973-84C9B618A1A8}" name="Percentage Increase vs Plaintext2" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{F4080A86-E0E6-428D-9973-84C9B618A1A8}" name="Percentage Increase vs Plaintext2" dataDxfId="3">
       <calculatedColumnFormula>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{30A9C073-FC8D-4D3E-B3F4-A25F0535FC84}" name="Eval Key Size (kB)" dataDxfId="14">
+    <tableColumn id="5" xr3:uid="{30A9C073-FC8D-4D3E-B3F4-A25F0535FC84}" name="Eval Key Size (kB)" dataDxfId="2">
       <calculatedColumnFormula>0.023</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9EE40A62-0BC7-4513-9103-444B1C53E933}" name="Private Key Size (kB)" dataDxfId="13">
+    <tableColumn id="6" xr3:uid="{9EE40A62-0BC7-4513-9103-444B1C53E933}" name="Private Key Size (kB)" dataDxfId="1">
       <calculatedColumnFormula>(Table4[[#This Row],[Run no.]]/Table4[[#This Row],[Percentage Increase vs Plaintext2]])*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{76F80D93-0ED4-416C-92DC-DF581C4F806B}" name="Increase in size vs RSA Standard" dataDxfId="12">
+    <tableColumn id="8" xr3:uid="{76F80D93-0ED4-416C-92DC-DF581C4F806B}" name="Increase in size vs RSA Standard" dataDxfId="0">
       <calculatedColumnFormula>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -979,24 +987,24 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{921BAE21-4B96-4F12-A7A8-47BA9506F67C}" name="Table578" displayName="Table578" ref="F2:I12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{921BAE21-4B96-4F12-A7A8-47BA9506F67C}" name="Table578" displayName="Table578" ref="F2:I12" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="F2:I12" xr:uid="{921BAE21-4B96-4F12-A7A8-47BA9506F67C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{97A1ECBF-985D-4294-89E3-45BDAA49FAAD}" name="Linear Regression" dataDxfId="9" dataCellStyle="Percent"/>
-    <tableColumn id="2" xr3:uid="{F3A1317D-74D5-4E25-BF5E-D8D4B3C2EF7B}" name="Random Forest" dataDxfId="8" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{FB9C8954-66F5-4DE2-BE3E-4A8164D0FCB3}" name="SVC" dataDxfId="7" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{907A467A-FA21-4927-B99F-EE5170044BB4}" name="Logistic Regression" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{97A1ECBF-985D-4294-89E3-45BDAA49FAAD}" name="Linear Regression" dataDxfId="15" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{F3A1317D-74D5-4E25-BF5E-D8D4B3C2EF7B}" name="Random Forest" dataDxfId="14" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{FB9C8954-66F5-4DE2-BE3E-4A8164D0FCB3}" name="SVC" dataDxfId="13" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{907A467A-FA21-4927-B99F-EE5170044BB4}" name="Logistic Regression" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{06850F0F-1F82-486C-991A-803478B128DC}" name="Table8" displayName="Table8" ref="F22:G33" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{06850F0F-1F82-486C-991A-803478B128DC}" name="Table8" displayName="Table8" ref="F22:G33" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="F22:G33" xr:uid="{06850F0F-1F82-486C-991A-803478B128DC}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E69931A7-7281-4236-B5F1-8FA661C967FE}" name="run no." dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{8C071A2A-7EC5-49A2-87BF-5DD99FB58EDF}" name="compilation time in seconds" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{E69931A7-7281-4236-B5F1-8FA661C967FE}" name="run no." dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{8C071A2A-7EC5-49A2-87BF-5DD99FB58EDF}" name="compilation time in seconds" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1267,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:M41"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="G4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16:J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1288,13 +1296,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="45"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="32"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -1303,62 +1311,62 @@
       <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="31" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="33"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="33"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="31" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="33"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="30"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="33"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="30"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="31" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="33"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="30"/>
     </row>
     <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="19" t="s">
         <v>54</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1400,204 +1408,204 @@
       <c r="M14" s="36"/>
     </row>
     <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="18" t="str">
+      <c r="E15" s="15" t="str">
         <f>"entire test set (" &amp; unit &amp; ")"</f>
         <v>entire test set (nanoseconds)</v>
       </c>
-      <c r="F15" s="18" t="str">
+      <c r="F15" s="15" t="str">
         <f>"average per-sample time (" &amp; unit &amp; ")"</f>
         <v>average per-sample time (nanoseconds)</v>
       </c>
-      <c r="G15" s="19" t="str">
+      <c r="G15" s="16" t="str">
         <f>"training time (" &amp; unit &amp; ")"</f>
         <v>training time (nanoseconds)</v>
       </c>
-      <c r="H15" s="19" t="str">
+      <c r="H15" s="16" t="str">
         <f>"quantization time (" &amp; unit &amp; ")"</f>
         <v>quantization time (nanoseconds)</v>
       </c>
-      <c r="I15" s="20" t="s">
+      <c r="I15" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J15" s="20" t="s">
+      <c r="J15" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K15" s="20" t="s">
+      <c r="K15" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="L15" s="20" t="s">
+      <c r="L15" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="M15" s="28" t="s">
+      <c r="M15" s="25" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="22">
         <f>AVERAGE('scikit-learn'!A3:A21)</f>
-        <v>0.98830803822372082</v>
-      </c>
-      <c r="C16" s="27">
+        <v>0.99280494659921248</v>
+      </c>
+      <c r="C16" s="24">
         <f>AVERAGE('scikit-learn'!B3:B12)</f>
-        <v>0.99658827633862868</v>
-      </c>
-      <c r="D16" s="25">
+        <v>0.99987875679382865</v>
+      </c>
+      <c r="D16" s="22">
         <f>AVERAGE(Table1[recall_score])/100</f>
-        <v>0.98746479999999992</v>
-      </c>
-      <c r="E16" s="27">
+        <v>0.9920178999999999</v>
+      </c>
+      <c r="E16" s="24">
         <f>AVERAGE(Table1[test_set_prediction_time])*micromultiplier</f>
         <v>267052.65045165969</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="24">
         <f>E16/$A$21</f>
         <v>150.1139125641707</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="24">
         <f>AVERAGE(Table1[training_time])*micromultiplier</f>
         <v>95986247.062682837</v>
       </c>
-      <c r="H16" s="27" t="s">
+      <c r="H16" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="I16" s="26">
+      <c r="I16" s="23">
         <f>ABS(B16-$B$16)</f>
         <v>0</v>
       </c>
-      <c r="J16" s="26">
+      <c r="J16" s="23">
         <f>ABS(1-C16/$C$16)</f>
         <v>0</v>
       </c>
-      <c r="K16" s="26">
+      <c r="K16" s="23">
         <f>ABS(1-E16/$E$16)</f>
         <v>0</v>
       </c>
-      <c r="L16" s="26">
+      <c r="L16" s="23">
         <f>ABS(1-(G16/$G$16))</f>
         <v>0</v>
       </c>
-      <c r="M16" s="14" t="str">
+      <c r="M16" s="12" t="str">
         <f xml:space="preserve"> ROUND((K16),2) &amp; "x slower"</f>
         <v>0x slower</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="25">
+      <c r="B17" s="22">
         <f>AVERAGE('quantized plaintext'!A3:A12)</f>
-        <v>0.98735244519392873</v>
-      </c>
-      <c r="C17" s="27">
+        <v>0.99252388982574458</v>
+      </c>
+      <c r="C17" s="24">
         <f>AVERAGE('quantized plaintext'!B3:B12)</f>
-        <v>0.99657517421600195</v>
-      </c>
-      <c r="D17" s="25">
+        <v>0.99987700524278522</v>
+      </c>
+      <c r="D17" s="22">
         <f>AVERAGE(Table2[recall_score])/100</f>
-        <v>0.98656560000000015</v>
-      </c>
-      <c r="E17" s="27">
+        <v>0.99213029999999991</v>
+      </c>
+      <c r="E17" s="24">
         <f>AVERAGE(Table2[test_set_prediction_time])*micromultiplier</f>
         <v>819325.44708251744</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F17" s="24">
         <f t="shared" ref="F17:F18" si="0">E17/$A$21</f>
         <v>460.55393315487208</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="24">
         <f>AVERAGE(Table2[training_time])*micromultiplier</f>
         <v>115684342.3843382</v>
       </c>
-      <c r="H17" s="27">
+      <c r="H17" s="24">
         <f>G17-$G$16</f>
         <v>19698095.321655363</v>
       </c>
-      <c r="I17" s="26">
+      <c r="I17" s="23">
         <f>ABS(B17-$B$16)</f>
-        <v>9.5559302979209004E-4</v>
-      </c>
-      <c r="J17" s="26">
+        <v>2.8105677346790259E-4</v>
+      </c>
+      <c r="J17" s="23">
         <f>ABS(1-C17/$C$16)</f>
-        <v>1.3146976477473871E-5</v>
-      </c>
-      <c r="K17" s="26">
+        <v>1.7517634328667597E-6</v>
+      </c>
+      <c r="K17" s="23">
         <f>ABS(1-E17/$E$16)</f>
         <v>2.068029640210693</v>
       </c>
-      <c r="L17" s="26">
+      <c r="L17" s="23">
         <f>ABS(1-(G17/$G$16))</f>
         <v>0.20521789240068666</v>
       </c>
-      <c r="M17" s="14" t="str">
+      <c r="M17" s="12" t="str">
         <f t="shared" ref="M17:M18" si="1" xml:space="preserve"> ROUND((K17),2) &amp; "x slower"</f>
         <v>2.07x slower</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="25">
+      <c r="B18" s="22">
         <f>AVERAGE('fhe (+ sizes)'!A3:A12)</f>
-        <v>0.98724002248454146</v>
-      </c>
-      <c r="C18" s="27">
+        <v>0.99252388982574458</v>
+      </c>
+      <c r="C18" s="24">
         <f>AVERAGE('fhe (+ sizes)'!B3:B12)</f>
-        <v>0.9965799561046621</v>
-      </c>
-      <c r="D18" s="25">
+        <v>0.99987700524278522</v>
+      </c>
+      <c r="D18" s="22">
         <f>AVERAGE(Table3[recall_score])/100</f>
-        <v>0.98594709999999997</v>
-      </c>
-      <c r="E18" s="27">
+        <v>0.99213029999999991</v>
+      </c>
+      <c r="E18" s="24">
         <f>AVERAGE(Table3[test_set_prediction_time])*micromultiplier</f>
         <v>955438.61389159935</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="24">
         <f t="shared" si="0"/>
         <v>537.06498813468204</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="24">
         <f>AVERAGE(Table2[training_time])*micromultiplier</f>
         <v>115684342.3843382</v>
       </c>
-      <c r="H18" s="27">
+      <c r="H18" s="24">
         <f>G18-$G$16</f>
         <v>19698095.321655363</v>
       </c>
-      <c r="I18" s="26">
+      <c r="I18" s="23">
         <f>ABS(B18-$B$16)</f>
-        <v>1.0680157391793621E-3</v>
-      </c>
-      <c r="J18" s="26">
+        <v>2.8105677346790259E-4</v>
+      </c>
+      <c r="J18" s="23">
         <f>ABS(1-C18/$C$16)</f>
-        <v>8.3487174835639166E-6</v>
-      </c>
-      <c r="K18" s="26">
+        <v>1.7517634328667597E-6</v>
+      </c>
+      <c r="K18" s="23">
         <f>ABS(1-E18/$E$16)</f>
         <v>2.5777162753325578</v>
       </c>
-      <c r="L18" s="26">
+      <c r="L18" s="23">
         <f>ABS(1-(G18/$G$16))</f>
         <v>0.20521789240068666</v>
       </c>
-      <c r="M18" s="14" t="str">
+      <c r="M18" s="12" t="str">
         <f t="shared" si="1"/>
         <v>2.58x slower</v>
       </c>
@@ -1611,25 +1619,25 @@
       <c r="A21" s="4">
         <v>1779</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J21" s="11" t="s">
+      <c r="J21" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K21" s="11" t="s">
+      <c r="K21" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="L21" s="11" t="s">
+      <c r="L21" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="M21" s="9"/>
+      <c r="M21" s="7"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="10" t="s">
+      <c r="I22" s="8" t="s">
         <v>45</v>
       </c>
       <c r="J22" s="1" t="str">
@@ -1649,7 +1657,7 @@
       <c r="A23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I23" s="10" t="s">
+      <c r="I23" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J23" s="1" t="str">
@@ -1666,7 +1674,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I24" s="10" t="s">
+      <c r="I24" s="8" t="s">
         <v>47</v>
       </c>
       <c r="J24" s="1" t="str">
@@ -1703,19 +1711,19 @@
       <c r="A26" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="25">
+      <c r="B26" s="22">
         <f>AVERAGE(Table5[Linear Regression])</f>
         <v>0.95924138668155945</v>
       </c>
-      <c r="C26" s="25">
+      <c r="C26" s="22">
         <f>AVERAGE(Table5[Random Forest])</f>
         <v>0.9871275997751543</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D26" s="22">
         <f>AVERAGE(Table5[SVC])</f>
         <v>0.98499156829679568</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E26" s="22">
         <f>AVERAGE(Table5[Logistic Regression])</f>
         <v>0.98802698145025247</v>
       </c>
@@ -1724,19 +1732,19 @@
       <c r="A27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="25">
+      <c r="B27" s="22">
         <f>AVERAGE(Table57[Linear Regression])</f>
         <v>0.95945015062941796</v>
       </c>
-      <c r="C27" s="25">
+      <c r="C27" s="22">
         <f>AVERAGE(Table57[Random Forest])</f>
         <v>0.98038223721191642</v>
       </c>
-      <c r="D27" s="25">
+      <c r="D27" s="22">
         <f>AVERAGE(Table57[SVC])</f>
         <v>0.98566610455311943</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="22">
         <f>AVERAGE(Table57[Logistic Regression])</f>
         <v>0.98560989319842562</v>
       </c>
@@ -1745,19 +1753,19 @@
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="25">
+      <c r="B28" s="22">
         <f>AVERAGE(Table578[Linear Regression])</f>
         <v>0.95795991505585998</v>
       </c>
-      <c r="C28" s="25">
+      <c r="C28" s="22">
         <f>AVERAGE(Table578[Random Forest])</f>
         <v>0.98116919617762766</v>
       </c>
-      <c r="D28" s="25">
+      <c r="D28" s="22">
         <f>AVERAGE(Table578[SVC])</f>
         <v>0.98555368184373204</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="22">
         <f>AVERAGE(Table578[Logistic Regression])</f>
         <v>0.98718381112984799</v>
       </c>
@@ -1871,6 +1879,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="I14:M14"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="B14:D14"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="A6:B6"/>
@@ -1879,14 +1895,6 @@
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="I14:M14"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="B14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1942,10 +1950,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>0.98763350196739697</v>
+        <v>0.98931984260820605</v>
       </c>
       <c r="B3" s="1">
-        <v>0.99660712684762598</v>
+        <v>0.99984221459359701</v>
       </c>
       <c r="C3" s="1">
         <v>2.13384628295898E-4</v>
@@ -1953,28 +1961,28 @@
       <c r="D3" s="1">
         <v>0.117744445800781</v>
       </c>
-      <c r="E3" s="23">
-        <v>98.594700000000003</v>
-      </c>
-      <c r="G3" s="13">
+      <c r="E3" s="20">
+        <v>99.156800000000004</v>
+      </c>
+      <c r="G3" s="11">
         <v>0.96652752901043792</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="11">
         <v>0.98819561551433399</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="11">
         <v>0.98819561551433399</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="11">
         <v>0.98650927487352402</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>0.98819561551433399</v>
+        <v>0.98763350196739697</v>
       </c>
       <c r="B4" s="1">
-        <v>0.996539459835875</v>
+        <v>0.99988389200837302</v>
       </c>
       <c r="C4" s="1">
         <v>4.2676925659179601E-4</v>
@@ -1982,28 +1990,28 @@
       <c r="D4" s="1">
         <v>0.11230659484863199</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="20">
         <v>98.932000000000002</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="11">
         <v>0.96029980379644098</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="11">
         <v>0.98650927487352402</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="11">
         <v>0.98482293423271505</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="11">
         <v>0.98988195615514296</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>0.98819561551433399</v>
+        <v>0.99381675098369804</v>
       </c>
       <c r="B5" s="1">
-        <v>0.99656215130963099</v>
+        <v>0.99989088743254495</v>
       </c>
       <c r="C5" s="1">
         <v>3.5905838012695302E-4</v>
@@ -2011,28 +2019,28 @@
       <c r="D5" s="1">
         <v>0.14333224296569799</v>
       </c>
-      <c r="E5" s="23">
-        <v>98.707099999999997</v>
-      </c>
-      <c r="G5" s="13">
+      <c r="E5" s="20">
+        <v>99.1006</v>
+      </c>
+      <c r="G5" s="11">
         <v>0.96139864520914997</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="11">
         <v>0.98875772906127002</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="11">
         <v>0.98819561551433399</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="11">
         <v>0.98538504777965097</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>0.98988195615514296</v>
+        <v>0.99269252388982498</v>
       </c>
       <c r="B6" s="1">
-        <v>0.99648901165327697</v>
+        <v>0.99988913910205302</v>
       </c>
       <c r="C6" s="1">
         <v>1.9264221191406201E-4</v>
@@ -2040,28 +2048,28 @@
       <c r="D6" s="1">
         <v>7.5737237930297796E-2</v>
       </c>
-      <c r="E6" s="23">
-        <v>98.650899999999993</v>
-      </c>
-      <c r="G6" s="13">
+      <c r="E6" s="20">
+        <v>98.988200000000006</v>
+      </c>
+      <c r="G6" s="11">
         <v>0.95935903472976802</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="11">
         <v>0.985947161326588</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="11">
         <v>0.98482293423271505</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="11">
         <v>0.98426082068577803</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>0.98763350196739697</v>
+        <v>0.99381675098369804</v>
       </c>
       <c r="B7" s="1">
-        <v>0.99660461352584695</v>
+        <v>0.99986954652501403</v>
       </c>
       <c r="C7" s="1">
         <v>2.5749206542968701E-4</v>
@@ -2069,28 +2077,28 @@
       <c r="D7" s="1">
         <v>8.4540605545043904E-2</v>
       </c>
-      <c r="E7" s="23">
-        <v>98.594700000000003</v>
-      </c>
-      <c r="G7" s="13">
+      <c r="E7" s="20">
+        <v>99.212999999999994</v>
+      </c>
+      <c r="G7" s="11">
         <v>0.95770520266258796</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="11">
         <v>0.98875772906127002</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="11">
         <v>0.98875772906127002</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="11">
         <v>0.98819561551433399</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>0.98988195615514296</v>
+        <v>0.99437886453063495</v>
       </c>
       <c r="B8" s="1">
-        <v>0.99659926717143699</v>
+        <v>0.99988254442379199</v>
       </c>
       <c r="C8" s="1">
         <v>1.8930435180664E-4</v>
@@ -2098,28 +2106,28 @@
       <c r="D8" s="1">
         <v>7.9212427139282199E-2</v>
       </c>
-      <c r="E8" s="23">
-        <v>98.707099999999997</v>
-      </c>
-      <c r="G8" s="13">
+      <c r="E8" s="20">
+        <v>99.325500000000005</v>
+      </c>
+      <c r="G8" s="11">
         <v>0.964341530725211</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="11">
         <v>0.99044406970207899</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="11">
         <v>0.99044406970207899</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="11">
         <v>0.98875772906127002</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>0.98707138842046005</v>
+        <v>0.99606520517144403</v>
       </c>
       <c r="B9" s="1">
-        <v>0.99667628669468999</v>
+        <v>0.99989327781329296</v>
       </c>
       <c r="C9" s="1">
         <v>2.6893615722656201E-4</v>
@@ -2127,28 +2135,28 @@
       <c r="D9" s="1">
         <v>7.4156761169433594E-2</v>
       </c>
-      <c r="E9" s="23">
-        <v>98.875799999999998</v>
-      </c>
-      <c r="G9" s="13">
+      <c r="E9" s="20">
+        <v>99.156800000000004</v>
+      </c>
+      <c r="G9" s="11">
         <v>0.95578470765438495</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="11">
         <v>0.98650927487352402</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="11">
         <v>0.97807757166947695</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="11">
         <v>0.98875772906127002</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>0.98988195615514296</v>
+        <v>0.99381675098369804</v>
       </c>
       <c r="B10" s="1">
-        <v>0.996591862758198</v>
+        <v>0.99988482137337198</v>
       </c>
       <c r="C10" s="1">
         <v>2.5749206542968701E-4</v>
@@ -2156,28 +2164,28 @@
       <c r="D10" s="1">
         <v>8.7489604949951102E-2</v>
       </c>
-      <c r="E10" s="23">
-        <v>98.875799999999998</v>
-      </c>
-      <c r="G10" s="13">
+      <c r="E10" s="20">
+        <v>99.494100000000003</v>
+      </c>
+      <c r="G10" s="11">
         <v>0.95698545829318504</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="11">
         <v>0.98426082068577803</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="11">
         <v>0.98088813940415909</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="11">
         <v>0.99100618324901601</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>0.98538504777965097</v>
+        <v>0.99213041034288896</v>
       </c>
       <c r="B11" s="1">
-        <v>0.99660694710886499</v>
+        <v>0.999892894054901</v>
       </c>
       <c r="C11" s="1">
         <v>2.5749206542968701E-4</v>
@@ -2185,28 +2193,28 @@
       <c r="D11" s="1">
         <v>0.10050606727600001</v>
       </c>
-      <c r="E11" s="23">
-        <v>98.875799999999998</v>
-      </c>
-      <c r="G11" s="13">
+      <c r="E11" s="20">
+        <v>99.550299999999993</v>
+      </c>
+      <c r="G11" s="11">
         <v>0.95597144180278204</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="11">
         <v>0.983698707138842</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="11">
         <v>0.98088813940415909</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="11">
         <v>0.98931984260820593</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>0.98931984260820605</v>
+        <v>0.99437886453063495</v>
       </c>
       <c r="B12" s="1">
-        <v>0.99660603648084101</v>
+        <v>0.99985835061134698</v>
       </c>
       <c r="C12" s="1">
         <v>2.47955322265625E-4</v>
@@ -2214,19 +2222,19 @@
       <c r="D12" s="1">
         <v>8.4836483001708901E-2</v>
       </c>
-      <c r="E12" s="23">
-        <v>98.650899999999993</v>
-      </c>
-      <c r="G12" s="13">
+      <c r="E12" s="20">
+        <v>99.1006</v>
+      </c>
+      <c r="G12" s="11">
         <v>0.95404051293164405</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="11">
         <v>0.98819561551433399</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="11">
         <v>0.98482293423271505</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="11">
         <v>0.98819561551433399</v>
       </c>
     </row>
@@ -2272,7 +2280,7 @@
   <dimension ref="A2:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E3" sqref="E3:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2313,10 +2321,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>0.98819561551433399</v>
+        <v>0.99213041034288896</v>
       </c>
       <c r="B3" s="1">
-        <v>0.99657174033290596</v>
+        <v>0.99983194630817696</v>
       </c>
       <c r="C3" s="1">
         <v>1.3179779052734299E-3</v>
@@ -2324,28 +2332,28 @@
       <c r="D3" s="1">
         <v>0.111749172210693</v>
       </c>
-      <c r="E3" s="23">
-        <v>98.932000000000002</v>
-      </c>
-      <c r="G3" s="13">
+      <c r="E3" s="20">
+        <v>99.156800000000004</v>
+      </c>
+      <c r="G3" s="11">
         <v>0.95997803717366392</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="11">
         <v>0.97976391231028603</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="11">
         <v>0.97976391231028603</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="11">
         <v>0.98032602585722306</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>0.99044406970207899</v>
+        <v>0.99100618324901601</v>
       </c>
       <c r="B4" s="1">
-        <v>0.99652743139232003</v>
+        <v>0.99988386568438103</v>
       </c>
       <c r="C4" s="1">
         <v>5.3310394287109299E-4</v>
@@ -2353,28 +2361,28 @@
       <c r="D4" s="1">
         <v>0.113413095474243</v>
       </c>
-      <c r="E4" s="23">
-        <v>99.044399999999996</v>
-      </c>
-      <c r="G4" s="13">
+      <c r="E4" s="20">
+        <v>99.437899999999999</v>
+      </c>
+      <c r="G4" s="11">
         <v>0.95842923781901701</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="11">
         <v>0.97920179876335001</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="11">
         <v>0.98538504777965097</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="11">
         <v>0.98538504777965097</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>0.98482293423271505</v>
+        <v>0.99325463743676201</v>
       </c>
       <c r="B5" s="1">
-        <v>0.99653276753727205</v>
+        <v>0.99987256206915598</v>
       </c>
       <c r="C5" s="1">
         <v>6.0558319091796799E-4</v>
@@ -2382,28 +2390,28 @@
       <c r="D5" s="1">
         <v>0.11999559402465799</v>
       </c>
-      <c r="E5" s="23">
-        <v>98.538499999999999</v>
-      </c>
-      <c r="G5" s="13">
+      <c r="E5" s="20">
+        <v>99.437899999999999</v>
+      </c>
+      <c r="G5" s="11">
         <v>0.95701969105871398</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="11">
         <v>0.98032602585722306</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="11">
         <v>0.98650927487352402</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="11">
         <v>0.98482293423271505</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>0.98482293423271505</v>
+        <v>0.99325463743676201</v>
       </c>
       <c r="B6" s="1">
-        <v>0.99659048559881303</v>
+        <v>0.99988623111630504</v>
       </c>
       <c r="C6" s="1">
         <v>6.9093704223632802E-4</v>
@@ -2411,28 +2419,28 @@
       <c r="D6" s="1">
         <v>0.11184048652648899</v>
       </c>
-      <c r="E6" s="23">
-        <v>98.369900000000001</v>
-      </c>
-      <c r="G6" s="13">
+      <c r="E6" s="20">
+        <v>99.212999999999994</v>
+      </c>
+      <c r="G6" s="11">
         <v>0.95909963293793898</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="11">
         <v>0.98088813940415909</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="11">
         <v>0.98482293423271505</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="11">
         <v>0.98426082068577803</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>0.99213041034288896</v>
+        <v>0.99325463743676201</v>
       </c>
       <c r="B7" s="1">
-        <v>0.99666277271553005</v>
+        <v>0.99989227224200095</v>
       </c>
       <c r="C7" s="1">
         <v>6.3920021057128895E-4</v>
@@ -2440,28 +2448,28 @@
       <c r="D7" s="1">
         <v>0.129948616027832</v>
       </c>
-      <c r="E7" s="23">
-        <v>98.482299999999995</v>
-      </c>
-      <c r="G7" s="13">
+      <c r="E7" s="20">
+        <v>98.875799999999998</v>
+      </c>
+      <c r="G7" s="11">
         <v>0.95349917927456107</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="11">
         <v>0.97807757166947695</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="11">
         <v>0.983698707138842</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="11">
         <v>0.98763350196739697</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>0.98707138842046005</v>
+        <v>0.99156829679595204</v>
       </c>
       <c r="B8" s="1">
-        <v>0.99650088119889901</v>
+        <v>0.99984127247493404</v>
       </c>
       <c r="C8" s="1">
         <v>9.7990036010742101E-4</v>
@@ -2469,28 +2477,28 @@
       <c r="D8" s="1">
         <v>0.10836601257324199</v>
       </c>
-      <c r="E8" s="23">
-        <v>98.650899999999993</v>
-      </c>
-      <c r="G8" s="13">
+      <c r="E8" s="20">
+        <v>99.156800000000004</v>
+      </c>
+      <c r="G8" s="11">
         <v>0.95887065391174209</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="11">
         <v>0.97751545812253993</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="11">
         <v>0.98819561551433399</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="11">
         <v>0.98931984260820593</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>0.98650927487352402</v>
+        <v>0.99325463743676201</v>
       </c>
       <c r="B9" s="1">
-        <v>0.99660454739990001</v>
+        <v>0.99989311154324401</v>
       </c>
       <c r="C9" s="1">
         <v>5.5932998657226497E-4</v>
@@ -2498,28 +2506,28 @@
       <c r="D9" s="1">
         <v>0.110030174255371</v>
       </c>
-      <c r="E9" s="23">
-        <v>98.763400000000004</v>
-      </c>
-      <c r="G9" s="13">
+      <c r="E9" s="20">
+        <v>99.156800000000004</v>
+      </c>
+      <c r="G9" s="11">
         <v>0.96203478051793989</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="11">
         <v>0.98088813940415909</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="11">
         <v>0.98538504777965097</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="11">
         <v>0.98201236649803203</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>0.98538504777965097</v>
+        <v>0.98931984260820605</v>
       </c>
       <c r="B10" s="1">
-        <v>0.99660680906766097</v>
+        <v>0.99989061691072001</v>
       </c>
       <c r="C10" s="1">
         <v>1.8444061279296799E-3</v>
@@ -2527,28 +2535,28 @@
       <c r="D10" s="1">
         <v>0.114490270614624</v>
       </c>
-      <c r="E10" s="23">
-        <v>98.875799999999998</v>
-      </c>
-      <c r="G10" s="13">
+      <c r="E10" s="20">
+        <v>99.212999999999994</v>
+      </c>
+      <c r="G10" s="11">
         <v>0.96075355421110298</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="11">
         <v>0.981450252951096</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="11">
         <v>0.985947161326588</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="11">
         <v>0.98707138842046005</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>0.98707138842046005</v>
+        <v>0.99269252388982498</v>
       </c>
       <c r="B11" s="1">
-        <v>0.99657438962837896</v>
+        <v>0.99988758629519703</v>
       </c>
       <c r="C11" s="1">
         <v>5.2356719970703103E-4</v>
@@ -2556,28 +2564,28 @@
       <c r="D11" s="1">
         <v>0.117451429367065</v>
       </c>
-      <c r="E11" s="23">
-        <v>98.369900000000001</v>
-      </c>
-      <c r="G11" s="13">
+      <c r="E11" s="20">
+        <v>99.269300000000001</v>
+      </c>
+      <c r="G11" s="11">
         <v>0.96345034945251096</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="11">
         <v>0.983698707138842</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="11">
         <v>0.98763350196739697</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="11">
         <v>0.98819561551433399</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>0.98707138842046005</v>
+        <v>0.99550309162450801</v>
       </c>
       <c r="B12" s="1">
-        <v>0.99657991728833994</v>
+        <v>0.99989058778373896</v>
       </c>
       <c r="C12" s="1">
         <v>4.9924850463867101E-4</v>
@@ -2585,76 +2593,76 @@
       <c r="D12" s="1">
         <v>0.119558572769165</v>
       </c>
-      <c r="E12" s="23">
-        <v>98.538499999999999</v>
-      </c>
-      <c r="G12" s="13">
+      <c r="E12" s="20">
+        <v>99.212999999999994</v>
+      </c>
+      <c r="G12" s="11">
         <v>0.96136638993698798</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="11">
         <v>0.98201236649803203</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="11">
         <v>0.98931984260820593</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="11">
         <v>0.98707138842046005</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2669,8 +2677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199A48B2-ACE2-47BC-9446-650C2E182FA4}">
   <dimension ref="A2:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2680,6 +2688,7 @@
     <col min="5" max="5" width="38.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -2710,24 +2719,24 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>0.98819561551433399</v>
+        <v>0.99213041034288896</v>
       </c>
       <c r="B3" s="1">
-        <v>0.99653155843004304</v>
+        <v>0.99983194630817696</v>
       </c>
       <c r="C3" s="1">
         <v>7.5984001159667904E-4</v>
       </c>
       <c r="D3" s="1">
-        <v>98.369900000000001</v>
-      </c>
-      <c r="F3" s="13">
+        <v>99.156800000000004</v>
+      </c>
+      <c r="F3" s="11">
         <v>0.96159279246192397</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="11">
         <v>0.983698707138842</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="11">
         <v>0.99100618324901601</v>
       </c>
       <c r="I3" s="2">
@@ -2736,24 +2745,24 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>0.99044406970207899</v>
+        <v>0.99100618324901601</v>
       </c>
       <c r="B4" s="1">
-        <v>0.99660196498589804</v>
+        <v>0.99988386568438103</v>
       </c>
       <c r="C4" s="1">
         <v>2.1140575408935499E-3</v>
       </c>
       <c r="D4" s="1">
-        <v>98.2012</v>
-      </c>
-      <c r="F4" s="13">
+        <v>99.437899999999999</v>
+      </c>
+      <c r="F4" s="11">
         <v>0.95350728877238788</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="11">
         <v>0.97695334457560401</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="11">
         <v>0.97751545812253993</v>
       </c>
       <c r="I4" s="2">
@@ -2762,24 +2771,24 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>0.98707138842046005</v>
+        <v>0.99325463743676201</v>
       </c>
       <c r="B5" s="1">
-        <v>0.99666767677517998</v>
+        <v>0.99987256206915598</v>
       </c>
       <c r="C5" s="1">
         <v>6.7448616027831999E-4</v>
       </c>
       <c r="D5" s="1">
-        <v>98.988200000000006</v>
-      </c>
-      <c r="F5" s="13">
+        <v>99.437899999999999</v>
+      </c>
+      <c r="F5" s="11">
         <v>0.95156378670129993</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="11">
         <v>0.97751545812253993</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="11">
         <v>0.98088813940415909</v>
       </c>
       <c r="I5" s="2">
@@ -2788,24 +2797,24 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>0.98988195615514296</v>
+        <v>0.99325463743676201</v>
       </c>
       <c r="B6" s="1">
-        <v>0.99660903268127699</v>
+        <v>0.99988623111630504</v>
       </c>
       <c r="C6" s="1">
         <v>6.7448616027831999E-4</v>
       </c>
       <c r="D6" s="1">
-        <v>98.932000000000002</v>
-      </c>
-      <c r="F6" s="13">
+        <v>99.212999999999994</v>
+      </c>
+      <c r="F6" s="11">
         <v>0.96393576246082202</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="11">
         <v>0.98426082068577803</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="11">
         <v>0.98819561551433399</v>
       </c>
       <c r="I6" s="2">
@@ -2814,24 +2823,24 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>0.98707138842046005</v>
+        <v>0.99325463743676201</v>
       </c>
       <c r="B7" s="1">
-        <v>0.99653169075208703</v>
+        <v>0.99989227224200095</v>
       </c>
       <c r="C7" s="1">
         <v>1.2099742889404199E-3</v>
       </c>
       <c r="D7" s="1">
-        <v>98.650899999999993</v>
-      </c>
-      <c r="F7" s="13">
+        <v>98.875799999999998</v>
+      </c>
+      <c r="F7" s="11">
         <v>0.95530617162711706</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="11">
         <v>0.97920179876335001</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="11">
         <v>0.98650927487352402</v>
       </c>
       <c r="I7" s="2">
@@ -2840,24 +2849,24 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>0.98707138842046005</v>
+        <v>0.99156829679595204</v>
       </c>
       <c r="B8" s="1">
-        <v>0.99659848924094396</v>
+        <v>0.99984127247493404</v>
       </c>
       <c r="C8" s="1">
         <v>7.5864791870117101E-4</v>
       </c>
       <c r="D8" s="1">
-        <v>98.426100000000005</v>
-      </c>
-      <c r="F8" s="13">
+        <v>99.156800000000004</v>
+      </c>
+      <c r="F8" s="11">
         <v>0.9607069777794589</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="11">
         <v>0.98650927487352402</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="11">
         <v>0.98763350196739697</v>
       </c>
       <c r="I8" s="2">
@@ -2866,24 +2875,24 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>0.983698707138842</v>
+        <v>0.99325463743676201</v>
       </c>
       <c r="B9" s="1">
-        <v>0.99660801160079904</v>
+        <v>0.99989311154324401</v>
       </c>
       <c r="C9" s="1">
         <v>9.1624259948730404E-4</v>
       </c>
       <c r="D9" s="1">
-        <v>98.594700000000003</v>
-      </c>
-      <c r="F9" s="13">
+        <v>99.156800000000004</v>
+      </c>
+      <c r="F9" s="11">
         <v>0.95271991445098902</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="11">
         <v>0.97920179876335001</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="11">
         <v>0.98482293423271505</v>
       </c>
       <c r="I9" s="2">
@@ -2892,24 +2901,24 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>0.98763350196739697</v>
+        <v>0.98931984260820605</v>
       </c>
       <c r="B10" s="1">
-        <v>0.99656921943556998</v>
+        <v>0.99989061691072001</v>
       </c>
       <c r="C10" s="1">
         <v>7.1120262145995996E-4</v>
       </c>
       <c r="D10" s="1">
-        <v>98.482299999999995</v>
-      </c>
-      <c r="F10" s="13">
+        <v>99.212999999999994</v>
+      </c>
+      <c r="F10" s="11">
         <v>0.9587638382913779</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="11">
         <v>0.97976391231028603</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="11">
         <v>0.98426082068577803</v>
       </c>
       <c r="I10" s="2">
@@ -2918,24 +2927,24 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>0.98538504777965097</v>
+        <v>0.99269252388982498</v>
       </c>
       <c r="B11" s="1">
-        <v>0.99652108207930901</v>
+        <v>0.99988758629519703</v>
       </c>
       <c r="C11" s="1">
         <v>6.7281723022460905E-4</v>
       </c>
       <c r="D11" s="1">
-        <v>98.707099999999997</v>
-      </c>
-      <c r="F11" s="13">
+        <v>99.269300000000001</v>
+      </c>
+      <c r="F11" s="11">
         <v>0.96335111688341202</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="11">
         <v>0.98482293423271505</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="11">
         <v>0.99044406970207899</v>
       </c>
       <c r="I11" s="2">
@@ -2944,24 +2953,24 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>0.985947161326588</v>
+        <v>0.99550309162450801</v>
       </c>
       <c r="B12" s="1">
-        <v>0.99656083506551396</v>
+        <v>0.99989058778373896</v>
       </c>
       <c r="C12" s="1">
         <v>1.0626316070556599E-3</v>
       </c>
       <c r="D12" s="1">
-        <v>98.594700000000003</v>
-      </c>
-      <c r="F12" s="13">
+        <v>99.212999999999994</v>
+      </c>
+      <c r="F12" s="11">
         <v>0.95815150112981096</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="11">
         <v>0.97976391231028603</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="11">
         <v>0.98426082068577803</v>
       </c>
       <c r="I12" s="2">
@@ -3004,28 +3013,28 @@
       <c r="B15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="20">
         <v>0.29399999999999998</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="20">
         <v>200.197</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="44">
         <f>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</f>
         <v>532.85866666666664</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="20">
         <f>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</f>
         <v>68094.217687074837</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="20">
         <f t="shared" ref="G15" si="0">0.023</f>
         <v>2.3E-2</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="20">
         <v>4</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="47">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
         <v>9.4166666666666661</v>
       </c>
@@ -3037,27 +3046,27 @@
       <c r="B16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="20">
         <v>0.29299999999999998</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="20">
         <v>200.197</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="44">
         <f>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</f>
         <v>532.85866666666664</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="20">
         <f>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</f>
         <v>68326.621160409559</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="20">
         <v>2.3E-2</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="20">
         <v>4</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="47">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
         <v>9.4166666666666661</v>
       </c>
@@ -3069,27 +3078,27 @@
       <c r="B17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="20">
         <v>0.29399999999999998</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="20">
         <v>200.197</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="44">
         <f>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</f>
         <v>532.85866666666664</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="20">
         <f>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</f>
         <v>68094.217687074837</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="20">
         <v>2.3E-2</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="20">
         <v>4</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="47">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
         <v>9.4166666666666661</v>
       </c>
@@ -3101,27 +3110,27 @@
       <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="20">
         <v>0.29699999999999999</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="20">
         <v>200.197</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="44">
         <f>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</f>
         <v>532.85866666666664</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="20">
         <f>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</f>
         <v>67406.39730639731</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="20">
         <v>2.3E-2</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="20">
         <v>4</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="47">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
         <v>9.4166666666666661</v>
       </c>
@@ -3133,27 +3142,27 @@
       <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="20">
         <v>0.29499999999999998</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="20">
         <v>200.197</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="44">
         <f>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</f>
         <v>532.85866666666664</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="20">
         <f>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</f>
         <v>67863.389830508488</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="20">
         <v>2.3E-2</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="20">
         <v>4</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="47">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
         <v>9.4166666666666661</v>
       </c>
@@ -3165,43 +3174,43 @@
       <c r="B20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="46">
         <f>AVERAGE(C15:C19)</f>
         <v>0.29459999999999997</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="46">
         <f t="shared" ref="D20:H20" si="1">AVERAGE(D15:D19)</f>
         <v>200.197</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="45">
         <f>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</f>
         <v>532.85866666666664</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="46">
         <f t="shared" si="1"/>
         <v>67956.968734293012</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="46">
         <f t="shared" si="1"/>
         <v>2.3E-2</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="46">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="49">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
         <v>9.4166666666666661</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="13" t="s">
         <v>65</v>
       </c>
       <c r="F22" s="5" t="s">
@@ -3215,11 +3224,11 @@
       <c r="B23" s="1">
         <v>3072</v>
       </c>
-      <c r="C23" s="16">
+      <c r="C23" s="48">
         <f>B23/8000</f>
         <v>0.38400000000000001</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="48">
         <v>0.375</v>
       </c>
       <c r="F23" s="1">

</xml_diff>

<commit_message>
combined features and classes files
</commit_message>
<xml_diff>
--- a/ML_Model_Scripts/Performance Data/New performance data.xlsx
+++ b/ML_Model_Scripts/Performance Data/New performance data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\vivs\Documents\concreteml-covid-classifier\ML_Model_Scripts\Performance Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8326644E-A926-4658-BD9C-EF05824DAEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8949F8BF-EF90-4547-834E-9F6A49E9873E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
   <si>
     <t>Plaintext</t>
   </si>
@@ -139,12 +139,6 @@
   </si>
   <si>
     <t>Run no.</t>
-  </si>
-  <si>
-    <t>Plaintext Size (kB)</t>
-  </si>
-  <si>
-    <t>Ciphertext Size (kB)</t>
   </si>
   <si>
     <t>Eval Key Size (kB)</t>
@@ -242,13 +236,22 @@
     <t>compilation time in nanoseconds</t>
   </si>
   <si>
-    <t>RSA Ciphertext Size (in kB)</t>
-  </si>
-  <si>
-    <t>Percentage Increase vs Plaintext2</t>
-  </si>
-  <si>
     <t>Percentage Increase vs RSA Ciphertext</t>
+  </si>
+  <si>
+    <t>128-bit security RSA Private Key File Size (in kB)</t>
+  </si>
+  <si>
+    <t>RSA Ciphertext File Size (in kB)</t>
+  </si>
+  <si>
+    <t>Ciphertext File Size (kB)</t>
+  </si>
+  <si>
+    <t>Plaintext File Size (kB)</t>
+  </si>
+  <si>
+    <t>Percentage Increase vs Plaintext</t>
   </si>
 </sst>
 </file>
@@ -256,10 +259,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="165" formatCode="0.0000%"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.000000%"/>
-    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000000%"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -478,46 +481,64 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -542,52 +563,34 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -597,34 +600,23 @@
   </cellStyles>
   <dxfs count="57">
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.0000%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0000%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -659,10 +651,68 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -671,30 +721,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -705,10 +731,29 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -721,25 +766,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -750,29 +776,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
+      <numFmt numFmtId="165" formatCode="0.0000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -939,46 +943,46 @@
     <tableColumn id="1" xr3:uid="{E9413FF7-271E-469E-BCC5-DC52D55F3A3A}" name="Linear Regression" dataDxfId="30" dataCellStyle="Percent"/>
     <tableColumn id="2" xr3:uid="{D6DB89F1-F914-4459-8D10-40E13FB298B0}" name="Random Forest" dataDxfId="29" dataCellStyle="Percent"/>
     <tableColumn id="3" xr3:uid="{C4F7B31F-A9DC-4D0B-B72F-83D8E4B839D1}" name="SVC" dataDxfId="28" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{546CB1C7-04D1-48CD-81F4-0F71D956336F}" name="Logistic Regression" dataDxfId="27" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{546CB1C7-04D1-48CD-81F4-0F71D956336F}" name="Logistic Regression" dataDxfId="4" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{274CBF2D-66AB-4A51-A1D7-B37000717CE9}" name="Table3" displayName="Table3" ref="A2:D12" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{274CBF2D-66AB-4A51-A1D7-B37000717CE9}" name="Table3" displayName="Table3" ref="A2:D12" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A2:D12" xr:uid="{274CBF2D-66AB-4A51-A1D7-B37000717CE9}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CF2700D2-A674-464D-946D-1F615B6D91A7}" name="accuracy" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{2EA8A39C-2C3A-4F0F-9292-AEF706305A49}" name="roc_auc_score" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{C2D54946-E516-44E8-911A-9CDEC9118CD9}" name="test_set_prediction_time" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{32534789-56F1-416C-9548-79FD73103C70}" name="recall_score" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{CF2700D2-A674-464D-946D-1F615B6D91A7}" name="accuracy" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{2EA8A39C-2C3A-4F0F-9292-AEF706305A49}" name="roc_auc_score" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{C2D54946-E516-44E8-911A-9CDEC9118CD9}" name="test_set_prediction_time" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{32534789-56F1-416C-9548-79FD73103C70}" name="recall_score" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E5D7C54E-16E1-4754-8032-313998CAF65E}" name="Table4" displayName="Table4" ref="A14:I20" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E5D7C54E-16E1-4754-8032-313998CAF65E}" name="Table4" displayName="Table4" ref="A14:I20" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A14:I20" xr:uid="{E5D7C54E-16E1-4754-8032-313998CAF65E}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E078801A-15C7-4980-8156-8BD235967CEF}" name="Run no." dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{EFC1765B-5F55-4EA2-8F83-E8A7E7C44F75}" name="Strain" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{F62F3C7A-45AD-49AC-B959-B08E20AA523B}" name="Plaintext Size (kB)" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{C782FB93-D156-4C46-B517-3AE650180077}" name="Ciphertext Size (kB)" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{9BA734C7-F6A6-4FCB-BB59-8D1BDD20BF6A}" name="Percentage Increase vs RSA Ciphertext" dataDxfId="4" dataCellStyle="Percent">
-      <calculatedColumnFormula>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{E078801A-15C7-4980-8156-8BD235967CEF}" name="Run no." dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{EFC1765B-5F55-4EA2-8F83-E8A7E7C44F75}" name="Strain" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{F62F3C7A-45AD-49AC-B959-B08E20AA523B}" name="Plaintext File Size (kB)" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{C782FB93-D156-4C46-B517-3AE650180077}" name="Ciphertext File Size (kB)" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{9BA734C7-F6A6-4FCB-BB59-8D1BDD20BF6A}" name="Percentage Increase vs RSA Ciphertext" dataDxfId="15" dataCellStyle="Percent">
+      <calculatedColumnFormula>ABS(1-Table4[[#This Row],[Ciphertext File Size (kB)]]/$D$23)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F4080A86-E0E6-428D-9973-84C9B618A1A8}" name="Percentage Increase vs Plaintext2" dataDxfId="3">
-      <calculatedColumnFormula>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{F4080A86-E0E6-428D-9973-84C9B618A1A8}" name="Percentage Increase vs Plaintext" dataDxfId="14">
+      <calculatedColumnFormula>(Table4[[#This Row],[Ciphertext File Size (kB)]]/Table4[[#This Row],[Plaintext File Size (kB)]])*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{30A9C073-FC8D-4D3E-B3F4-A25F0535FC84}" name="Eval Key Size (kB)" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{30A9C073-FC8D-4D3E-B3F4-A25F0535FC84}" name="Eval Key Size (kB)" dataDxfId="13">
       <calculatedColumnFormula>0.023</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9EE40A62-0BC7-4513-9103-444B1C53E933}" name="Private Key Size (kB)" dataDxfId="1">
-      <calculatedColumnFormula>(Table4[[#This Row],[Run no.]]/Table4[[#This Row],[Percentage Increase vs Plaintext2]])*100</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{9EE40A62-0BC7-4513-9103-444B1C53E933}" name="Private Key Size (kB)" dataDxfId="12">
+      <calculatedColumnFormula>(Table4[[#This Row],[Run no.]]/Table4[[#This Row],[Percentage Increase vs Plaintext]])*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{76F80D93-0ED4-416C-92DC-DF581C4F806B}" name="Increase in size vs RSA Standard" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{76F80D93-0ED4-416C-92DC-DF581C4F806B}" name="Increase in size vs RSA Standard" dataDxfId="11">
       <calculatedColumnFormula>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -987,24 +991,24 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{921BAE21-4B96-4F12-A7A8-47BA9506F67C}" name="Table578" displayName="Table578" ref="F2:I12" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{921BAE21-4B96-4F12-A7A8-47BA9506F67C}" name="Table578" displayName="Table578" ref="F2:I12" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="F2:I12" xr:uid="{921BAE21-4B96-4F12-A7A8-47BA9506F67C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{97A1ECBF-985D-4294-89E3-45BDAA49FAAD}" name="Linear Regression" dataDxfId="15" dataCellStyle="Percent"/>
-    <tableColumn id="2" xr3:uid="{F3A1317D-74D5-4E25-BF5E-D8D4B3C2EF7B}" name="Random Forest" dataDxfId="14" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{FB9C8954-66F5-4DE2-BE3E-4A8164D0FCB3}" name="SVC" dataDxfId="13" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{907A467A-FA21-4927-B99F-EE5170044BB4}" name="Logistic Regression" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{97A1ECBF-985D-4294-89E3-45BDAA49FAAD}" name="Linear Regression" dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{F3A1317D-74D5-4E25-BF5E-D8D4B3C2EF7B}" name="Random Forest" dataDxfId="1" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{FB9C8954-66F5-4DE2-BE3E-4A8164D0FCB3}" name="SVC" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{907A467A-FA21-4927-B99F-EE5170044BB4}" name="Logistic Regression" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{06850F0F-1F82-486C-991A-803478B128DC}" name="Table8" displayName="Table8" ref="F22:G33" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{06850F0F-1F82-486C-991A-803478B128DC}" name="Table8" displayName="Table8" ref="F22:G33" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="F22:G33" xr:uid="{06850F0F-1F82-486C-991A-803478B128DC}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E69931A7-7281-4236-B5F1-8FA661C967FE}" name="run no." dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{8C071A2A-7EC5-49A2-87BF-5DD99FB58EDF}" name="compilation time in seconds" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{E69931A7-7281-4236-B5F1-8FA661C967FE}" name="run no." dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{8C071A2A-7EC5-49A2-87BF-5DD99FB58EDF}" name="compilation time in seconds" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1275,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16:J18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1296,13 +1300,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="38"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -1311,66 +1315,66 @@
       <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="28" t="s">
+      <c r="B4" s="33"/>
+      <c r="C4" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30"/>
+      <c r="A5" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="33"/>
+      <c r="C5" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="35"/>
+      <c r="E5" s="36"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28" t="s">
+      <c r="B6" s="33"/>
+      <c r="C6" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="30"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="36"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="28" t="s">
+      <c r="B7" s="33"/>
+      <c r="C7" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="30"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="36"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="28" t="s">
+      <c r="B8" s="33"/>
+      <c r="C8" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="36"/>
     </row>
     <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C10" s="4">
         <f>IF(ISNUMBER(SEARCH("nano", unit)),1000000000, 1000000)</f>
@@ -1378,34 +1382,34 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="38" t="str">
+      <c r="C14" s="48"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="44" t="str">
         <f xml:space="preserve"> "running time (" &amp; unit &amp; ")"</f>
         <v>running time (nanoseconds)</v>
       </c>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="34" t="s">
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="36"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="42"/>
     </row>
     <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
@@ -1418,7 +1422,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E15" s="15" t="str">
         <f>"entire test set (" &amp; unit &amp; ")"</f>
@@ -1443,13 +1447,13 @@
         <v>9</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M15" s="25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -1481,7 +1485,7 @@
         <v>95986247.062682837</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I16" s="23">
         <f>ABS(B16-$B$16)</f>
@@ -1620,16 +1624,16 @@
         <v>1779</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J21" s="9" t="s">
         <v>11</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M21" s="7"/>
     </row>
@@ -1638,7 +1642,7 @@
         <v>23</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J22" s="1" t="str">
         <f>ROUND(ABS(1-(E17/$E$16)),2) &amp; "x slower"</f>
@@ -1658,7 +1662,7 @@
         <v>24</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J23" s="1" t="str">
         <f>ROUND(ABS(1-(E18/$E$16)),2) &amp; "x slower"</f>
@@ -1675,7 +1679,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I24" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J24" s="1" t="str">
         <f>ROUND(ABS(1-(E18/$E$17)),2) &amp; "x slower"</f>
@@ -1713,19 +1717,19 @@
       </c>
       <c r="B26" s="22">
         <f>AVERAGE(Table5[Linear Regression])</f>
-        <v>0.95924138668155945</v>
+        <v>0.95309590636527286</v>
       </c>
       <c r="C26" s="22">
         <f>AVERAGE(Table5[Random Forest])</f>
-        <v>0.9871275997751543</v>
+        <v>0.99505340078695848</v>
       </c>
       <c r="D26" s="22">
         <f>AVERAGE(Table5[SVC])</f>
-        <v>0.98499156829679568</v>
+        <v>0.99066891512085387</v>
       </c>
       <c r="E26" s="22">
         <f>AVERAGE(Table5[Logistic Regression])</f>
-        <v>0.98802698145025247</v>
+        <v>0.99280494659921248</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -1734,19 +1738,19 @@
       </c>
       <c r="B27" s="22">
         <f>AVERAGE(Table57[Linear Regression])</f>
-        <v>0.95945015062941796</v>
+        <v>0.95315661887599923</v>
       </c>
       <c r="C27" s="22">
         <f>AVERAGE(Table57[Random Forest])</f>
-        <v>0.98038223721191642</v>
+        <v>0.99072512647554767</v>
       </c>
       <c r="D27" s="22">
         <f>AVERAGE(Table57[SVC])</f>
-        <v>0.98566610455311943</v>
+        <v>0.9914558740865651</v>
       </c>
       <c r="E27" s="22">
         <f>AVERAGE(Table57[Logistic Regression])</f>
-        <v>0.98560989319842562</v>
+        <v>0.99252388982574458</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -1755,27 +1759,27 @@
       </c>
       <c r="B28" s="22">
         <f>AVERAGE(Table578[Linear Regression])</f>
-        <v>0.95795991505585998</v>
+        <v>0.95315661887599923</v>
       </c>
       <c r="C28" s="22">
         <f>AVERAGE(Table578[Random Forest])</f>
-        <v>0.98116919617762766</v>
+        <v>0.99072512647554767</v>
       </c>
       <c r="D28" s="22">
         <f>AVERAGE(Table578[SVC])</f>
-        <v>0.98555368184373204</v>
+        <v>0.9914558740865651</v>
       </c>
       <c r="E28" s="22">
         <f>AVERAGE(Table578[Logistic Regression])</f>
-        <v>0.98718381112984799</v>
+        <v>0.99252388982574458</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -1870,7 +1874,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B41" s="1">
         <f>'fhe (+ sizes)'!G33*micromultiplier</f>
@@ -1908,8 +1912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{866B64C5-BF1A-499D-83A6-EB0DDBB99A75}">
   <dimension ref="A2:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E12"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1933,7 +1937,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>27</v>
@@ -1965,16 +1969,16 @@
         <v>99.156800000000004</v>
       </c>
       <c r="G3" s="11">
-        <v>0.96652752901043792</v>
+        <v>0.95598401269285105</v>
       </c>
       <c r="H3" s="11">
-        <v>0.98819561551433399</v>
+        <v>0.99437886453063495</v>
       </c>
       <c r="I3" s="11">
-        <v>0.98819561551433399</v>
+        <v>0.99325463743676201</v>
       </c>
       <c r="J3" s="11">
-        <v>0.98650927487352402</v>
+        <v>0.98931984260820605</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1994,16 +1998,16 @@
         <v>98.932000000000002</v>
       </c>
       <c r="G4" s="11">
-        <v>0.96029980379644098</v>
+        <v>0.96035730568184996</v>
       </c>
       <c r="H4" s="11">
-        <v>0.98650927487352402</v>
+        <v>0.99606520517144403</v>
       </c>
       <c r="I4" s="11">
-        <v>0.98482293423271505</v>
+        <v>0.99100618324901601</v>
       </c>
       <c r="J4" s="11">
-        <v>0.98988195615514296</v>
+        <v>0.98763350196739697</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2023,16 +2027,16 @@
         <v>99.1006</v>
       </c>
       <c r="G5" s="11">
-        <v>0.96139864520914997</v>
+        <v>0.95406130708460202</v>
       </c>
       <c r="H5" s="11">
-        <v>0.98875772906127002</v>
+        <v>0.99550309162450801</v>
       </c>
       <c r="I5" s="11">
-        <v>0.98819561551433399</v>
+        <v>0.98931984260820605</v>
       </c>
       <c r="J5" s="11">
-        <v>0.98538504777965097</v>
+        <v>0.99381675098369804</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2052,16 +2056,16 @@
         <v>98.988200000000006</v>
       </c>
       <c r="G6" s="11">
-        <v>0.95935903472976802</v>
+        <v>0.953410087676971</v>
       </c>
       <c r="H6" s="11">
-        <v>0.985947161326588</v>
+        <v>0.99381675098369804</v>
       </c>
       <c r="I6" s="11">
-        <v>0.98482293423271505</v>
+        <v>0.99213041034288896</v>
       </c>
       <c r="J6" s="11">
-        <v>0.98426082068577803</v>
+        <v>0.99269252388982498</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2081,16 +2085,16 @@
         <v>99.212999999999994</v>
       </c>
       <c r="G7" s="11">
-        <v>0.95770520266258796</v>
+        <v>0.946978190475254</v>
       </c>
       <c r="H7" s="11">
-        <v>0.98875772906127002</v>
+        <v>0.99606520517144403</v>
       </c>
       <c r="I7" s="11">
-        <v>0.98875772906127002</v>
+        <v>0.98538504777965097</v>
       </c>
       <c r="J7" s="11">
-        <v>0.98819561551433399</v>
+        <v>0.99381675098369804</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -2110,16 +2114,16 @@
         <v>99.325500000000005</v>
       </c>
       <c r="G8" s="11">
-        <v>0.964341530725211</v>
+        <v>0.95047512087219999</v>
       </c>
       <c r="H8" s="11">
-        <v>0.99044406970207899</v>
+        <v>0.99662731871838095</v>
       </c>
       <c r="I8" s="11">
-        <v>0.99044406970207899</v>
+        <v>0.99381675098369804</v>
       </c>
       <c r="J8" s="11">
-        <v>0.98875772906127002</v>
+        <v>0.99437886453063495</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -2139,16 +2143,16 @@
         <v>99.156800000000004</v>
       </c>
       <c r="G9" s="11">
-        <v>0.95578470765438495</v>
+        <v>0.95401280152822598</v>
       </c>
       <c r="H9" s="11">
-        <v>0.98650927487352402</v>
+        <v>0.99550309162450801</v>
       </c>
       <c r="I9" s="11">
-        <v>0.97807757166947695</v>
+        <v>0.98988195615514296</v>
       </c>
       <c r="J9" s="11">
-        <v>0.98875772906127002</v>
+        <v>0.99606520517144403</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -2168,16 +2172,16 @@
         <v>99.494100000000003</v>
       </c>
       <c r="G10" s="11">
-        <v>0.95698545829318504</v>
+        <v>0.95363798530324195</v>
       </c>
       <c r="H10" s="11">
-        <v>0.98426082068577803</v>
+        <v>0.99550309162450801</v>
       </c>
       <c r="I10" s="11">
-        <v>0.98088813940415909</v>
+        <v>0.99269252388982498</v>
       </c>
       <c r="J10" s="11">
-        <v>0.99100618324901601</v>
+        <v>0.99381675098369804</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -2197,16 +2201,16 @@
         <v>99.550299999999993</v>
       </c>
       <c r="G11" s="11">
-        <v>0.95597144180278204</v>
+        <v>0.95400100133787902</v>
       </c>
       <c r="H11" s="11">
-        <v>0.983698707138842</v>
+        <v>0.99381675098369804</v>
       </c>
       <c r="I11" s="11">
-        <v>0.98088813940415909</v>
+        <v>0.99044406970207899</v>
       </c>
       <c r="J11" s="11">
-        <v>0.98931984260820593</v>
+        <v>0.99213041034288896</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -2226,16 +2230,16 @@
         <v>99.1006</v>
       </c>
       <c r="G12" s="11">
-        <v>0.95404051293164405</v>
+        <v>0.94804125099965297</v>
       </c>
       <c r="H12" s="11">
-        <v>0.98819561551433399</v>
+        <v>0.99325463743676201</v>
       </c>
       <c r="I12" s="11">
-        <v>0.98482293423271505</v>
+        <v>0.98875772906127002</v>
       </c>
       <c r="J12" s="11">
-        <v>0.98819561551433399</v>
+        <v>0.99437886453063495</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -2279,8 +2283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82957BC5-845A-415D-A9C1-AC076A441DA7}">
   <dimension ref="A2:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E12"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2304,7 +2308,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>27</v>
@@ -2336,16 +2340,16 @@
         <v>99.156800000000004</v>
       </c>
       <c r="G3" s="11">
-        <v>0.95997803717366392</v>
+        <v>0.95054265031858498</v>
       </c>
       <c r="H3" s="11">
-        <v>0.97976391231028603</v>
+        <v>0.98931984260820605</v>
       </c>
       <c r="I3" s="11">
-        <v>0.97976391231028603</v>
-      </c>
-      <c r="J3" s="11">
-        <v>0.98032602585722306</v>
+        <v>0.99100618324901601</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.99213041034288896</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -2365,16 +2369,16 @@
         <v>99.437899999999999</v>
       </c>
       <c r="G4" s="11">
-        <v>0.95842923781901701</v>
+        <v>0.949951992688576</v>
       </c>
       <c r="H4" s="11">
-        <v>0.97920179876335001</v>
+        <v>0.985947161326588</v>
       </c>
       <c r="I4" s="11">
-        <v>0.98538504777965097</v>
-      </c>
-      <c r="J4" s="11">
-        <v>0.98538504777965097</v>
+        <v>0.98931984260820605</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.99100618324901601</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2394,16 +2398,16 @@
         <v>99.437899999999999</v>
       </c>
       <c r="G5" s="11">
-        <v>0.95701969105871398</v>
+        <v>0.95044661591118595</v>
       </c>
       <c r="H5" s="11">
-        <v>0.98032602585722306</v>
+        <v>0.98931984260820605</v>
       </c>
       <c r="I5" s="11">
-        <v>0.98650927487352402</v>
-      </c>
-      <c r="J5" s="11">
-        <v>0.98482293423271505</v>
+        <v>0.99100618324901601</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.99325463743676201</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2423,16 +2427,16 @@
         <v>99.212999999999994</v>
       </c>
       <c r="G6" s="11">
-        <v>0.95909963293793898</v>
+        <v>0.95297910306760802</v>
       </c>
       <c r="H6" s="11">
-        <v>0.98088813940415909</v>
+        <v>0.99550309162450801</v>
       </c>
       <c r="I6" s="11">
-        <v>0.98482293423271505</v>
-      </c>
-      <c r="J6" s="11">
-        <v>0.98426082068577803</v>
+        <v>0.98988195615514296</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.99325463743676201</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2452,16 +2456,16 @@
         <v>98.875799999999998</v>
       </c>
       <c r="G7" s="11">
-        <v>0.95349917927456107</v>
+        <v>0.95254117242323699</v>
       </c>
       <c r="H7" s="11">
-        <v>0.97807757166947695</v>
+        <v>0.99100618324901601</v>
       </c>
       <c r="I7" s="11">
-        <v>0.983698707138842</v>
-      </c>
-      <c r="J7" s="11">
-        <v>0.98763350196739697</v>
+        <v>0.99437886453063495</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.99325463743676201</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -2481,16 +2485,16 @@
         <v>99.156800000000004</v>
       </c>
       <c r="G8" s="11">
-        <v>0.95887065391174209</v>
+        <v>0.94853862708822001</v>
       </c>
       <c r="H8" s="11">
-        <v>0.97751545812253993</v>
+        <v>0.98538504777965097</v>
       </c>
       <c r="I8" s="11">
-        <v>0.98819561551433399</v>
-      </c>
-      <c r="J8" s="11">
-        <v>0.98931984260820593</v>
+        <v>0.99100618324901601</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.99156829679595204</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -2510,16 +2514,16 @@
         <v>99.156800000000004</v>
       </c>
       <c r="G9" s="11">
-        <v>0.96203478051793989</v>
+        <v>0.96128788204707705</v>
       </c>
       <c r="H9" s="11">
-        <v>0.98088813940415909</v>
+        <v>0.99437886453063495</v>
       </c>
       <c r="I9" s="11">
-        <v>0.98538504777965097</v>
-      </c>
-      <c r="J9" s="11">
-        <v>0.98201236649803203</v>
+        <v>0.99269252388982498</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.99325463743676201</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -2539,16 +2543,16 @@
         <v>99.212999999999994</v>
       </c>
       <c r="G10" s="11">
-        <v>0.96075355421110298</v>
+        <v>0.95032258446400097</v>
       </c>
       <c r="H10" s="11">
-        <v>0.981450252951096</v>
+        <v>0.99325463743676201</v>
       </c>
       <c r="I10" s="11">
-        <v>0.985947161326588</v>
-      </c>
-      <c r="J10" s="11">
-        <v>0.98707138842046005</v>
+        <v>0.99325463743676201</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.98931984260820605</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -2568,16 +2572,16 @@
         <v>99.269300000000001</v>
       </c>
       <c r="G11" s="11">
-        <v>0.96345034945251096</v>
+        <v>0.95786047487711401</v>
       </c>
       <c r="H11" s="11">
-        <v>0.983698707138842</v>
+        <v>0.99269252388982498</v>
       </c>
       <c r="I11" s="11">
-        <v>0.98763350196739697</v>
-      </c>
-      <c r="J11" s="11">
-        <v>0.98819561551433399</v>
+        <v>0.99325463743676201</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.99269252388982498</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -2597,16 +2601,16 @@
         <v>99.212999999999994</v>
       </c>
       <c r="G12" s="11">
-        <v>0.96136638993698798</v>
+        <v>0.95709508587438996</v>
       </c>
       <c r="H12" s="11">
-        <v>0.98201236649803203</v>
+        <v>0.99044406970207899</v>
       </c>
       <c r="I12" s="11">
-        <v>0.98931984260820593</v>
-      </c>
-      <c r="J12" s="11">
-        <v>0.98707138842046005</v>
+        <v>0.98875772906127002</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.99550309162450801</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -2677,8 +2681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199A48B2-ACE2-47BC-9446-650C2E182FA4}">
   <dimension ref="A2:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2702,7 +2706,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>27</v>
@@ -2731,16 +2735,16 @@
         <v>99.156800000000004</v>
       </c>
       <c r="F3" s="11">
-        <v>0.96159279246192397</v>
+        <v>0.95054265031858498</v>
       </c>
       <c r="G3" s="11">
-        <v>0.983698707138842</v>
+        <v>0.98931984260820605</v>
       </c>
       <c r="H3" s="11">
         <v>0.99100618324901601</v>
       </c>
       <c r="I3" s="2">
-        <v>0.98763350196739697</v>
+        <v>0.99213041034288896</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -2757,16 +2761,16 @@
         <v>99.437899999999999</v>
       </c>
       <c r="F4" s="11">
-        <v>0.95350728877238788</v>
+        <v>0.949951992688576</v>
       </c>
       <c r="G4" s="11">
-        <v>0.97695334457560401</v>
+        <v>0.985947161326588</v>
       </c>
       <c r="H4" s="11">
-        <v>0.97751545812253993</v>
+        <v>0.98931984260820605</v>
       </c>
       <c r="I4" s="2">
-        <v>0.983698707138842</v>
+        <v>0.99100618324901601</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -2783,16 +2787,16 @@
         <v>99.437899999999999</v>
       </c>
       <c r="F5" s="11">
-        <v>0.95156378670129993</v>
+        <v>0.95044661591118595</v>
       </c>
       <c r="G5" s="11">
-        <v>0.97751545812253993</v>
+        <v>0.98931984260820605</v>
       </c>
       <c r="H5" s="11">
-        <v>0.98088813940415909</v>
+        <v>0.99100618324901601</v>
       </c>
       <c r="I5" s="2">
-        <v>0.98875772906127002</v>
+        <v>0.99325463743676201</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -2809,16 +2813,16 @@
         <v>99.212999999999994</v>
       </c>
       <c r="F6" s="11">
-        <v>0.96393576246082202</v>
+        <v>0.95297910306760802</v>
       </c>
       <c r="G6" s="11">
-        <v>0.98426082068577803</v>
+        <v>0.99550309162450801</v>
       </c>
       <c r="H6" s="11">
-        <v>0.98819561551433399</v>
+        <v>0.98988195615514296</v>
       </c>
       <c r="I6" s="2">
-        <v>0.98875772906127002</v>
+        <v>0.99325463743676201</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -2835,16 +2839,16 @@
         <v>98.875799999999998</v>
       </c>
       <c r="F7" s="11">
-        <v>0.95530617162711706</v>
+        <v>0.95254117242323699</v>
       </c>
       <c r="G7" s="11">
-        <v>0.97920179876335001</v>
+        <v>0.99100618324901601</v>
       </c>
       <c r="H7" s="11">
-        <v>0.98650927487352402</v>
+        <v>0.99437886453063495</v>
       </c>
       <c r="I7" s="2">
-        <v>0.98763350196739697</v>
+        <v>0.99325463743676201</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -2861,16 +2865,16 @@
         <v>99.156800000000004</v>
       </c>
       <c r="F8" s="11">
-        <v>0.9607069777794589</v>
+        <v>0.94853862708822001</v>
       </c>
       <c r="G8" s="11">
-        <v>0.98650927487352402</v>
+        <v>0.98538504777965097</v>
       </c>
       <c r="H8" s="11">
-        <v>0.98763350196739697</v>
+        <v>0.99100618324901601</v>
       </c>
       <c r="I8" s="2">
-        <v>0.98426082068577803</v>
+        <v>0.99156829679595204</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -2887,16 +2891,16 @@
         <v>99.156800000000004</v>
       </c>
       <c r="F9" s="11">
-        <v>0.95271991445098902</v>
+        <v>0.96128788204707705</v>
       </c>
       <c r="G9" s="11">
-        <v>0.97920179876335001</v>
+        <v>0.99437886453063495</v>
       </c>
       <c r="H9" s="11">
-        <v>0.98482293423271505</v>
+        <v>0.99269252388982498</v>
       </c>
       <c r="I9" s="2">
-        <v>0.98538504777965097</v>
+        <v>0.99325463743676201</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -2913,16 +2917,16 @@
         <v>99.212999999999994</v>
       </c>
       <c r="F10" s="11">
-        <v>0.9587638382913779</v>
+        <v>0.95032258446400097</v>
       </c>
       <c r="G10" s="11">
-        <v>0.97976391231028603</v>
+        <v>0.99325463743676201</v>
       </c>
       <c r="H10" s="11">
-        <v>0.98426082068577803</v>
+        <v>0.99325463743676201</v>
       </c>
       <c r="I10" s="2">
-        <v>0.98819561551433399</v>
+        <v>0.98931984260820605</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -2939,16 +2943,16 @@
         <v>99.269300000000001</v>
       </c>
       <c r="F11" s="11">
-        <v>0.96335111688341202</v>
+        <v>0.95786047487711401</v>
       </c>
       <c r="G11" s="11">
-        <v>0.98482293423271505</v>
+        <v>0.99269252388982498</v>
       </c>
       <c r="H11" s="11">
-        <v>0.99044406970207899</v>
+        <v>0.99325463743676201</v>
       </c>
       <c r="I11" s="2">
-        <v>0.98650927487352402</v>
+        <v>0.99269252388982498</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -2965,16 +2969,16 @@
         <v>99.212999999999994</v>
       </c>
       <c r="F12" s="11">
-        <v>0.95815150112981096</v>
+        <v>0.95709508587438996</v>
       </c>
       <c r="G12" s="11">
-        <v>0.97976391231028603</v>
+        <v>0.99044406970207899</v>
       </c>
       <c r="H12" s="11">
-        <v>0.98426082068577803</v>
+        <v>0.98875772906127002</v>
       </c>
       <c r="I12" s="2">
-        <v>0.99100618324901601</v>
+        <v>0.99550309162450801</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -2982,28 +2986,28 @@
         <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="I14" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -3011,21 +3015,21 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="20">
-        <v>0.29399999999999998</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="D15" s="20">
         <v>200.197</v>
       </c>
-      <c r="E15" s="44">
-        <f>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</f>
+      <c r="E15" s="26">
+        <f>ABS(1-Table4[[#This Row],[Ciphertext File Size (kB)]]/$D$23)</f>
         <v>532.85866666666664</v>
       </c>
       <c r="F15" s="20">
-        <f>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</f>
-        <v>68094.217687074837</v>
+        <f>(Table4[[#This Row],[Ciphertext File Size (kB)]]/Table4[[#This Row],[Plaintext File Size (kB)]])*100</f>
+        <v>465574.41860465123</v>
       </c>
       <c r="G15" s="20">
         <f t="shared" ref="G15" si="0">0.023</f>
@@ -3034,9 +3038,9 @@
       <c r="H15" s="20">
         <v>4</v>
       </c>
-      <c r="I15" s="47">
+      <c r="I15" s="29">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
-        <v>9.4166666666666661</v>
+        <v>0.65700082850041408</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -3044,21 +3048,21 @@
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C16" s="20">
-        <v>0.29299999999999998</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="D16" s="20">
         <v>200.197</v>
       </c>
-      <c r="E16" s="44">
-        <f>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</f>
+      <c r="E16" s="26">
+        <f>ABS(1-Table4[[#This Row],[Ciphertext File Size (kB)]]/$D$23)</f>
         <v>532.85866666666664</v>
       </c>
       <c r="F16" s="20">
-        <f>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</f>
-        <v>68326.621160409559</v>
+        <f>(Table4[[#This Row],[Ciphertext File Size (kB)]]/Table4[[#This Row],[Plaintext File Size (kB)]])*100</f>
+        <v>476659.52380952379</v>
       </c>
       <c r="G16" s="20">
         <v>2.3E-2</v>
@@ -3066,9 +3070,9 @@
       <c r="H16" s="20">
         <v>4</v>
       </c>
-      <c r="I16" s="47">
+      <c r="I16" s="29">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
-        <v>9.4166666666666661</v>
+        <v>0.65700082850041408</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -3076,21 +3080,21 @@
         <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C17" s="20">
-        <v>0.29399999999999998</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="D17" s="20">
         <v>200.197</v>
       </c>
-      <c r="E17" s="44">
-        <f>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</f>
+      <c r="E17" s="26">
+        <f>ABS(1-Table4[[#This Row],[Ciphertext File Size (kB)]]/$D$23)</f>
         <v>532.85866666666664</v>
       </c>
       <c r="F17" s="20">
-        <f>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</f>
-        <v>68094.217687074837</v>
+        <f>(Table4[[#This Row],[Ciphertext File Size (kB)]]/Table4[[#This Row],[Plaintext File Size (kB)]])*100</f>
+        <v>465574.41860465123</v>
       </c>
       <c r="G17" s="20">
         <v>2.3E-2</v>
@@ -3098,9 +3102,9 @@
       <c r="H17" s="20">
         <v>4</v>
       </c>
-      <c r="I17" s="47">
+      <c r="I17" s="29">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
-        <v>9.4166666666666661</v>
+        <v>0.65700082850041408</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -3108,21 +3112,21 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18" s="20">
-        <v>0.29699999999999999</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="D18" s="20">
         <v>200.197</v>
       </c>
-      <c r="E18" s="44">
-        <f>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</f>
+      <c r="E18" s="26">
+        <f>ABS(1-Table4[[#This Row],[Ciphertext File Size (kB)]]/$D$23)</f>
         <v>532.85866666666664</v>
       </c>
       <c r="F18" s="20">
-        <f>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</f>
-        <v>67406.39730639731</v>
+        <f>(Table4[[#This Row],[Ciphertext File Size (kB)]]/Table4[[#This Row],[Plaintext File Size (kB)]])*100</f>
+        <v>435210.86956521741</v>
       </c>
       <c r="G18" s="20">
         <v>2.3E-2</v>
@@ -3130,9 +3134,9 @@
       <c r="H18" s="20">
         <v>4</v>
       </c>
-      <c r="I18" s="47">
+      <c r="I18" s="29">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
-        <v>9.4166666666666661</v>
+        <v>0.65700082850041408</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -3140,21 +3144,21 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" s="20">
-        <v>0.29499999999999998</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="D19" s="20">
         <v>200.197</v>
       </c>
-      <c r="E19" s="44">
-        <f>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</f>
+      <c r="E19" s="26">
+        <f>ABS(1-Table4[[#This Row],[Ciphertext File Size (kB)]]/$D$23)</f>
         <v>532.85866666666664</v>
       </c>
       <c r="F19" s="20">
-        <f>(Table4[[#This Row],[Ciphertext Size (kB)]]/Table4[[#This Row],[Plaintext Size (kB)]])*100</f>
-        <v>67863.389830508488</v>
+        <f>(Table4[[#This Row],[Ciphertext File Size (kB)]]/Table4[[#This Row],[Plaintext File Size (kB)]])*100</f>
+        <v>454993.18181818188</v>
       </c>
       <c r="G19" s="20">
         <v>2.3E-2</v>
@@ -3162,73 +3166,79 @@
       <c r="H19" s="20">
         <v>4</v>
       </c>
-      <c r="I19" s="47">
+      <c r="I19" s="29">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
-        <v>9.4166666666666661</v>
+        <v>0.65700082850041408</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="46">
+        <v>40</v>
+      </c>
+      <c r="C20" s="28">
         <f>AVERAGE(C15:C19)</f>
-        <v>0.29459999999999997</v>
-      </c>
-      <c r="D20" s="46">
+        <v>4.3599999999999993E-2</v>
+      </c>
+      <c r="D20" s="28">
         <f t="shared" ref="D20:H20" si="1">AVERAGE(D15:D19)</f>
         <v>200.197</v>
       </c>
-      <c r="E20" s="45">
-        <f>ABS(1-Table4[[#This Row],[Ciphertext Size (kB)]]/$D$23)</f>
+      <c r="E20" s="27">
+        <f>ABS(1-Table4[[#This Row],[Ciphertext File Size (kB)]]/$D$23)</f>
         <v>532.85866666666664</v>
       </c>
-      <c r="F20" s="46">
+      <c r="F20" s="28">
         <f t="shared" si="1"/>
-        <v>67956.968734293012</v>
-      </c>
-      <c r="G20" s="46">
+        <v>459602.48248044512</v>
+      </c>
+      <c r="G20" s="28">
         <f t="shared" si="1"/>
         <v>2.3E-2</v>
       </c>
-      <c r="H20" s="46">
+      <c r="H20" s="28">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I20" s="49">
+      <c r="I20" s="31">
         <f>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</f>
-        <v>9.4166666666666661</v>
+        <v>0.65700082850041408</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="13" t="s">
+        <v>50</v>
+      </c>
       <c r="B22" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="D22" s="13" t="s">
         <v>65</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="1">
+      <c r="A23" s="1">
         <v>3072</v>
       </c>
-      <c r="C23" s="48">
-        <f>B23/8000</f>
+      <c r="B23" s="30">
+        <f>A23/8000</f>
         <v>0.38400000000000001</v>
       </c>
-      <c r="D23" s="48">
+      <c r="C23" s="30">
+        <v>2.4140000000000001</v>
+      </c>
+      <c r="D23" s="30">
         <v>0.375</v>
       </c>
       <c r="F23" s="1">
@@ -3239,6 +3249,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C24" s="20">
+        <v>2.4180000000000001</v>
+      </c>
       <c r="F24" s="1">
         <v>2</v>
       </c>
@@ -3247,8 +3260,8 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>58</v>
+      <c r="C25" s="30">
+        <v>2.4140000000000001</v>
       </c>
       <c r="F25" s="1">
         <v>3</v>
@@ -3258,6 +3271,9 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C26" s="30">
+        <v>2.4140000000000001</v>
+      </c>
       <c r="F26" s="1">
         <v>4</v>
       </c>
@@ -3266,6 +3282,9 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C27" s="20">
+        <v>2.4180000000000001</v>
+      </c>
       <c r="F27" s="1">
         <v>5</v>
       </c>
@@ -3274,6 +3293,10 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C28" s="28">
+        <f>AVERAGE(C23:C27)</f>
+        <v>2.4156</v>
+      </c>
       <c r="F28" s="1">
         <v>6</v>
       </c>
@@ -3282,6 +3305,9 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
       <c r="F29" s="1">
         <v>7</v>
       </c>
@@ -3315,7 +3341,7 @@
     </row>
     <row r="33" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F33" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G33" s="1">
         <f>AVERAGE(G23:G32)</f>

</xml_diff>

<commit_message>
added documents and user manual
</commit_message>
<xml_diff>
--- a/ML_Model_Scripts/Performance Data/New performance data.xlsx
+++ b/ML_Model_Scripts/Performance Data/New performance data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\vivs\Documents\concreteml-covid-classifier\ML_Model_Scripts\Performance Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E6810F-32B0-437F-87E0-819DC3523C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233F03F8-BE93-42A0-8ED8-8C77937C32B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
     <sheet name="scikit-learn" sheetId="2" r:id="rId2"/>
     <sheet name="quantized plaintext" sheetId="3" r:id="rId3"/>
     <sheet name="fhe (+ sizes)" sheetId="4" r:id="rId4"/>
+    <sheet name="fhe (nbits)" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="micromultiplier">Overall!$C$10</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
   <si>
     <t>Plaintext</t>
   </si>
@@ -252,6 +253,18 @@
   </si>
   <si>
     <t>Percentage Increase vs Plaintext</t>
+  </si>
+  <si>
+    <t>n_bits</t>
+  </si>
+  <si>
+    <t>Run 1</t>
+  </si>
+  <si>
+    <t>Run 2</t>
+  </si>
+  <si>
+    <t>Run 3</t>
   </si>
 </sst>
 </file>
@@ -554,6 +567,36 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -561,36 +604,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -598,25 +611,26 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="57">
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+  <dxfs count="63">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -648,6 +662,22 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -710,6 +740,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -883,11 +917,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E9CFD89E-23B4-4900-868A-D7C63CC3629E}" name="Table10" displayName="Table10" ref="A30:B41" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E9CFD89E-23B4-4900-868A-D7C63CC3629E}" name="Table10" displayName="Table10" ref="A30:B41" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
   <autoFilter ref="A30:B41" xr:uid="{E9CFD89E-23B4-4900-868A-D7C63CC3629E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FDD77692-0B2D-40D7-9D09-720C76DC1D39}" name="run no." dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{BE378DC4-90AA-4B9F-B636-DD04BF9D4413}" name="compilation time in nanoseconds" dataDxfId="53">
+    <tableColumn id="1" xr3:uid="{FDD77692-0B2D-40D7-9D09-720C76DC1D39}" name="run no." dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{BE378DC4-90AA-4B9F-B636-DD04BF9D4413}" name="compilation time in nanoseconds" dataDxfId="59">
       <calculatedColumnFormula>'fhe (+ sizes)'!G23*micromultiplier</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -895,94 +929,107 @@
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{820D2F3B-0C47-4C46-9289-47E4B41BED5E}" name="Table9" displayName="Table9" ref="A1:D16" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5">
+  <autoFilter ref="A1:D16" xr:uid="{820D2F3B-0C47-4C46-9289-47E4B41BED5E}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{DAB3CDEF-794A-4E82-9CB2-23CEA6265AA3}" name="n_bits" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{0E996090-D945-495F-95CD-C3E04409F46D}" name="Run 1" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{1BACCA03-9469-46AD-BCDE-84A8E6A2B964}" name="Run 2" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{957472DD-2190-4860-8F83-2F4FBCE21820}" name="Run 3" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{394116DB-3FC4-462F-A6EA-93CE28E8DEFC}" name="Table1" displayName="Table1" ref="A2:E12" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{394116DB-3FC4-462F-A6EA-93CE28E8DEFC}" name="Table1" displayName="Table1" ref="A2:E12" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="A2:E12" xr:uid="{394116DB-3FC4-462F-A6EA-93CE28E8DEFC}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{CFED003A-DA1B-4CE5-8524-E8936E3DBC3E}" name="accuracy" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{E1948511-7D29-400B-AA26-A9E601B91AEC}" name="roc_auc_score" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{7A51BA68-3B03-403B-89BD-9395BC2871EB}" name="test_set_prediction_time" dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{832497D3-116A-4DE3-A927-E67DAAF345F9}" name="training_time" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{6BF1096A-6B0A-4B1A-BD35-2A1207399D49}" name="recall_score" dataDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{CFED003A-DA1B-4CE5-8524-E8936E3DBC3E}" name="accuracy" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{E1948511-7D29-400B-AA26-A9E601B91AEC}" name="roc_auc_score" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{7A51BA68-3B03-403B-89BD-9395BC2871EB}" name="test_set_prediction_time" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{832497D3-116A-4DE3-A927-E67DAAF345F9}" name="training_time" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{6BF1096A-6B0A-4B1A-BD35-2A1207399D49}" name="recall_score" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4BDC63FC-A3D1-4A76-971A-2D7E1A53E2E0}" name="Table5" displayName="Table5" ref="G2:J12" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4BDC63FC-A3D1-4A76-971A-2D7E1A53E2E0}" name="Table5" displayName="Table5" ref="G2:J12" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="G2:J12" xr:uid="{4BDC63FC-A3D1-4A76-971A-2D7E1A53E2E0}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{590571B2-7F3A-4AB4-82F6-490D3ABC5319}" name="Linear Regression" dataDxfId="43" dataCellStyle="Percent"/>
-    <tableColumn id="2" xr3:uid="{07D40D9A-323F-4837-9150-E888FA1F58E4}" name="Random Forest" dataDxfId="42" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{852582AB-50FA-439E-807C-CDA24D4C70C4}" name="SVC" dataDxfId="41" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{799C5940-B5F5-4EC3-89E0-C94AD8F231A7}" name="Logistic Regression" dataDxfId="40" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{590571B2-7F3A-4AB4-82F6-490D3ABC5319}" name="Linear Regression" dataDxfId="49" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{07D40D9A-323F-4837-9150-E888FA1F58E4}" name="Random Forest" dataDxfId="48" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{852582AB-50FA-439E-807C-CDA24D4C70C4}" name="SVC" dataDxfId="47" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{799C5940-B5F5-4EC3-89E0-C94AD8F231A7}" name="Logistic Regression" dataDxfId="46" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{51C47605-6D87-4135-B9CB-CCDCB9C5785B}" name="Table2" displayName="Table2" ref="A2:E12" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{51C47605-6D87-4135-B9CB-CCDCB9C5785B}" name="Table2" displayName="Table2" ref="A2:E12" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
   <autoFilter ref="A2:E12" xr:uid="{51C47605-6D87-4135-B9CB-CCDCB9C5785B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D1463535-C8C0-4CDA-8D2E-CC2600120E02}" name="accuracy" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{B5EFEA31-5244-404F-A004-FB2C24EF05C5}" name="roc_auc_score" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{4ECC1606-A197-4F05-B01C-AE05A7881542}" name="test_set_prediction_time" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{5607816E-855A-4944-AF8F-D298454F5A6B}" name="training_time" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{6C282614-58D3-469E-8D4B-11E62AD2B121}" name="recall_score" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{D1463535-C8C0-4CDA-8D2E-CC2600120E02}" name="accuracy" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{B5EFEA31-5244-404F-A004-FB2C24EF05C5}" name="roc_auc_score" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{4ECC1606-A197-4F05-B01C-AE05A7881542}" name="test_set_prediction_time" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{5607816E-855A-4944-AF8F-D298454F5A6B}" name="training_time" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{6C282614-58D3-469E-8D4B-11E62AD2B121}" name="recall_score" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E7F5510B-26CB-48F1-9BD1-CC49FC0D68B6}" name="Table57" displayName="Table57" ref="G2:J12" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E7F5510B-26CB-48F1-9BD1-CC49FC0D68B6}" name="Table57" displayName="Table57" ref="G2:J12" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
   <autoFilter ref="G2:J12" xr:uid="{E7F5510B-26CB-48F1-9BD1-CC49FC0D68B6}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E9413FF7-271E-469E-BCC5-DC52D55F3A3A}" name="Linear Regression" dataDxfId="30" dataCellStyle="Percent"/>
-    <tableColumn id="2" xr3:uid="{D6DB89F1-F914-4459-8D10-40E13FB298B0}" name="Random Forest" dataDxfId="29" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{C4F7B31F-A9DC-4D0B-B72F-83D8E4B839D1}" name="SVC" dataDxfId="28" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{546CB1C7-04D1-48CD-81F4-0F71D956336F}" name="Logistic Regression" dataDxfId="4" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{E9413FF7-271E-469E-BCC5-DC52D55F3A3A}" name="Linear Regression" dataDxfId="36" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{D6DB89F1-F914-4459-8D10-40E13FB298B0}" name="Random Forest" dataDxfId="35" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{C4F7B31F-A9DC-4D0B-B72F-83D8E4B839D1}" name="SVC" dataDxfId="34" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{546CB1C7-04D1-48CD-81F4-0F71D956336F}" name="Logistic Regression" dataDxfId="33" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{274CBF2D-66AB-4A51-A1D7-B37000717CE9}" name="Table3" displayName="Table3" ref="A2:D12" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{274CBF2D-66AB-4A51-A1D7-B37000717CE9}" name="Table3" displayName="Table3" ref="A2:D12" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A2:D12" xr:uid="{274CBF2D-66AB-4A51-A1D7-B37000717CE9}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CF2700D2-A674-464D-946D-1F615B6D91A7}" name="accuracy" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{2EA8A39C-2C3A-4F0F-9292-AEF706305A49}" name="roc_auc_score" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{C2D54946-E516-44E8-911A-9CDEC9118CD9}" name="test_set_prediction_time" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{32534789-56F1-416C-9548-79FD73103C70}" name="recall_score" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{CF2700D2-A674-464D-946D-1F615B6D91A7}" name="accuracy" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{2EA8A39C-2C3A-4F0F-9292-AEF706305A49}" name="roc_auc_score" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{C2D54946-E516-44E8-911A-9CDEC9118CD9}" name="test_set_prediction_time" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{32534789-56F1-416C-9548-79FD73103C70}" name="recall_score" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E5D7C54E-16E1-4754-8032-313998CAF65E}" name="Table4" displayName="Table4" ref="A14:I20" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E5D7C54E-16E1-4754-8032-313998CAF65E}" name="Table4" displayName="Table4" ref="A14:I20" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A14:I20" xr:uid="{E5D7C54E-16E1-4754-8032-313998CAF65E}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E078801A-15C7-4980-8156-8BD235967CEF}" name="Run no." dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{EFC1765B-5F55-4EA2-8F83-E8A7E7C44F75}" name="Strain" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{F62F3C7A-45AD-49AC-B959-B08E20AA523B}" name="Plaintext File Size (kB)" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{C782FB93-D156-4C46-B517-3AE650180077}" name="Ciphertext File Size (kB)" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{9BA734C7-F6A6-4FCB-BB59-8D1BDD20BF6A}" name="Percentage Increase vs RSA Ciphertext" dataDxfId="15" dataCellStyle="Percent">
+    <tableColumn id="1" xr3:uid="{E078801A-15C7-4980-8156-8BD235967CEF}" name="Run no." dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{EFC1765B-5F55-4EA2-8F83-E8A7E7C44F75}" name="Strain" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{F62F3C7A-45AD-49AC-B959-B08E20AA523B}" name="Plaintext File Size (kB)" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{C782FB93-D156-4C46-B517-3AE650180077}" name="Ciphertext File Size (kB)" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{9BA734C7-F6A6-4FCB-BB59-8D1BDD20BF6A}" name="Percentage Increase vs RSA Ciphertext" dataDxfId="20" dataCellStyle="Percent">
       <calculatedColumnFormula>ABS(1-Table4[[#This Row],[Ciphertext File Size (kB)]]/$D$23)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F4080A86-E0E6-428D-9973-84C9B618A1A8}" name="Percentage Increase vs Plaintext" dataDxfId="14">
+    <tableColumn id="4" xr3:uid="{F4080A86-E0E6-428D-9973-84C9B618A1A8}" name="Percentage Increase vs Plaintext" dataDxfId="19">
       <calculatedColumnFormula>(Table4[[#This Row],[Ciphertext File Size (kB)]]/Table4[[#This Row],[Plaintext File Size (kB)]])*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{30A9C073-FC8D-4D3E-B3F4-A25F0535FC84}" name="Eval Key Size (kB)" dataDxfId="13">
+    <tableColumn id="5" xr3:uid="{30A9C073-FC8D-4D3E-B3F4-A25F0535FC84}" name="Eval Key Size (kB)" dataDxfId="18">
       <calculatedColumnFormula>0.023</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9EE40A62-0BC7-4513-9103-444B1C53E933}" name="Private Key Size (kB)" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{9EE40A62-0BC7-4513-9103-444B1C53E933}" name="Private Key Size (kB)" dataDxfId="17">
       <calculatedColumnFormula>(Table4[[#This Row],[Run no.]]/Table4[[#This Row],[Percentage Increase vs Plaintext]])*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{76F80D93-0ED4-416C-92DC-DF581C4F806B}" name="Increase in size vs RSA Standard" dataDxfId="11">
+    <tableColumn id="8" xr3:uid="{76F80D93-0ED4-416C-92DC-DF581C4F806B}" name="Increase in size vs RSA Standard" dataDxfId="16">
       <calculatedColumnFormula>ABS(1-(Table4[[#This Row],[Private Key Size (kB)]]/$C$23))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -991,24 +1038,24 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{921BAE21-4B96-4F12-A7A8-47BA9506F67C}" name="Table578" displayName="Table578" ref="F2:I12" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{921BAE21-4B96-4F12-A7A8-47BA9506F67C}" name="Table578" displayName="Table578" ref="F2:I12" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="F2:I12" xr:uid="{921BAE21-4B96-4F12-A7A8-47BA9506F67C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{97A1ECBF-985D-4294-89E3-45BDAA49FAAD}" name="Linear Regression" dataDxfId="2" dataCellStyle="Percent"/>
-    <tableColumn id="2" xr3:uid="{F3A1317D-74D5-4E25-BF5E-D8D4B3C2EF7B}" name="Random Forest" dataDxfId="1" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{FB9C8954-66F5-4DE2-BE3E-4A8164D0FCB3}" name="SVC" dataDxfId="0" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{907A467A-FA21-4927-B99F-EE5170044BB4}" name="Logistic Regression" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{97A1ECBF-985D-4294-89E3-45BDAA49FAAD}" name="Linear Regression" dataDxfId="13" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{F3A1317D-74D5-4E25-BF5E-D8D4B3C2EF7B}" name="Random Forest" dataDxfId="12" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{FB9C8954-66F5-4DE2-BE3E-4A8164D0FCB3}" name="SVC" dataDxfId="11" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{907A467A-FA21-4927-B99F-EE5170044BB4}" name="Logistic Regression" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{06850F0F-1F82-486C-991A-803478B128DC}" name="Table8" displayName="Table8" ref="F22:G33" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{06850F0F-1F82-486C-991A-803478B128DC}" name="Table8" displayName="Table8" ref="F22:G33" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="F22:G33" xr:uid="{06850F0F-1F82-486C-991A-803478B128DC}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E69931A7-7281-4236-B5F1-8FA661C967FE}" name="run no." dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{8C071A2A-7EC5-49A2-87BF-5DD99FB58EDF}" name="compilation time in seconds" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{E69931A7-7281-4236-B5F1-8FA661C967FE}" name="run no." dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{8C071A2A-7EC5-49A2-87BF-5DD99FB58EDF}" name="compilation time in seconds" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1300,13 +1347,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="38"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="48"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -1382,34 +1429,34 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="48"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="44" t="str">
+      <c r="C14" s="45"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="41" t="str">
         <f xml:space="preserve"> "running time (" &amp; unit &amp; ")"</f>
         <v>running time (nanoseconds)</v>
       </c>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="40" t="s">
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="42"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="39"/>
     </row>
     <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
@@ -1883,6 +1930,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="A8:B8"/>
@@ -1891,14 +1946,6 @@
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="E14:H14"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2681,7 +2728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199A48B2-ACE2-47BC-9446-650C2E182FA4}">
   <dimension ref="A2:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -3358,4 +3405,252 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17EAEC2D-8D3E-41C5-AF09-678F310E3372}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="4" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="29">
+        <v>0.48116900000000001</v>
+      </c>
+      <c r="C2" s="29">
+        <v>0.68746499999999999</v>
+      </c>
+      <c r="D2" s="29">
+        <v>0.66217000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="29">
+        <v>0.89038799999999996</v>
+      </c>
+      <c r="C3" s="29">
+        <v>0.978078</v>
+      </c>
+      <c r="D3" s="29">
+        <v>0.98650899999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="29">
+        <v>0.98988200000000004</v>
+      </c>
+      <c r="C4" s="29">
+        <v>0.99100600000000005</v>
+      </c>
+      <c r="D4" s="29">
+        <v>0.98707100000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+      <c r="B5" s="29">
+        <v>0.98988200000000004</v>
+      </c>
+      <c r="C5" s="29">
+        <v>0.99212999999999996</v>
+      </c>
+      <c r="D5" s="29">
+        <v>0.98931999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6" s="29">
+        <v>0.99212999999999996</v>
+      </c>
+      <c r="C6" s="29">
+        <v>0.991568</v>
+      </c>
+      <c r="D6" s="29">
+        <v>0.98988200000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>7</v>
+      </c>
+      <c r="B7" s="29">
+        <v>0.99269300000000005</v>
+      </c>
+      <c r="C7" s="29">
+        <v>0.99212999999999996</v>
+      </c>
+      <c r="D7" s="29">
+        <v>0.98875800000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>8</v>
+      </c>
+      <c r="B8" s="29">
+        <v>0.99269300000000005</v>
+      </c>
+      <c r="C8" s="29">
+        <v>0.99212999999999996</v>
+      </c>
+      <c r="D8" s="29">
+        <v>0.99044399999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>9</v>
+      </c>
+      <c r="B9" s="29">
+        <v>0.99269300000000005</v>
+      </c>
+      <c r="C9" s="29">
+        <v>0.99212999999999996</v>
+      </c>
+      <c r="D9" s="29">
+        <v>0.98988200000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>10</v>
+      </c>
+      <c r="B10" s="29">
+        <v>0.99269300000000005</v>
+      </c>
+      <c r="C10" s="29">
+        <v>0.99212999999999996</v>
+      </c>
+      <c r="D10" s="29">
+        <v>0.98988200000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>11</v>
+      </c>
+      <c r="B11" s="29">
+        <v>0.99269300000000005</v>
+      </c>
+      <c r="C11" s="29">
+        <v>0.99212999999999996</v>
+      </c>
+      <c r="D11" s="29">
+        <v>0.98988200000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>12</v>
+      </c>
+      <c r="B12" s="29">
+        <v>0.99269300000000005</v>
+      </c>
+      <c r="C12" s="29">
+        <v>0.99212999999999996</v>
+      </c>
+      <c r="D12" s="29">
+        <v>0.98988200000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>13</v>
+      </c>
+      <c r="B13" s="29">
+        <v>0.99269300000000005</v>
+      </c>
+      <c r="C13" s="29">
+        <v>0.99212999999999996</v>
+      </c>
+      <c r="D13" s="29">
+        <v>0.98988200000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>14</v>
+      </c>
+      <c r="B14" s="29">
+        <v>0.99269300000000005</v>
+      </c>
+      <c r="C14" s="29">
+        <v>0.99212999999999996</v>
+      </c>
+      <c r="D14" s="29">
+        <v>0.98988200000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>15</v>
+      </c>
+      <c r="B15" s="29">
+        <v>0.99269300000000005</v>
+      </c>
+      <c r="C15" s="29">
+        <v>0.99212999999999996</v>
+      </c>
+      <c r="D15" s="29">
+        <v>0.98988200000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>16</v>
+      </c>
+      <c r="B16" s="29">
+        <v>0.99269300000000005</v>
+      </c>
+      <c r="C16" s="29">
+        <v>0.99212999999999996</v>
+      </c>
+      <c r="D16" s="29">
+        <v>0.98988200000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>